<commit_message>
temporarily removed artists with minor song detail update
</commit_message>
<xml_diff>
--- a/music_list_7.xlsx
+++ b/music_list_7.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2476" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2479" uniqueCount="874">
   <si>
     <t>歌名</t>
   </si>
@@ -136,7 +136,7 @@
     <t>爱你不是两三天</t>
   </si>
   <si>
-    <t>爱你</t>
+    <t>王心凌 - 爱你</t>
   </si>
   <si>
     <t>王心凌</t>
@@ -2254,13 +2254,22 @@
     <t>自己按门铃自己听</t>
   </si>
   <si>
+    <t>周深</t>
+  </si>
+  <si>
     <t>17岁</t>
   </si>
   <si>
+    <t>刘德华</t>
+  </si>
+  <si>
     <t>粤语</t>
   </si>
   <si>
     <t>喜帖街</t>
+  </si>
+  <si>
+    <t>谢安琪</t>
   </si>
   <si>
     <t>大风吹</t>
@@ -2634,44 +2643,44 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="38">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
+    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
+    <numFmt numFmtId="177" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="178" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="179" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="180" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="181" formatCode="\¥#,##0;\¥\-#,##0"/>
+    <numFmt numFmtId="182" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="183" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="184" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="185" formatCode="yy/m/d"/>
+    <numFmt numFmtId="186" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
-    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
-    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
-    <numFmt numFmtId="178" formatCode="mmmm\-yy"/>
-    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="179" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="187" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="188" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="189" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="190" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="191" formatCode="mmmmm"/>
+    <numFmt numFmtId="192" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="193" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="194" formatCode="m/d"/>
+    <numFmt numFmtId="195" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="196" formatCode="mmmmm\-yy"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="180" formatCode="mmmmm"/>
-    <numFmt numFmtId="181" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="182" formatCode="#\ ??/??"/>
-    <numFmt numFmtId="183" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="197" formatCode="#\ ??/??"/>
+    <numFmt numFmtId="198" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="199" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
     <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="184" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="185" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="186" formatCode="yy/m/d"/>
-    <numFmt numFmtId="187" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="188" formatCode="m/d"/>
-    <numFmt numFmtId="189" formatCode="[$-804]aaa"/>
-    <numFmt numFmtId="190" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="191" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="192" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="193" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="200" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+    <numFmt numFmtId="201" formatCode="#\ ??"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="194" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="195" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="196" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="197" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="198" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="199" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="200" formatCode="#\ ??"/>
-    <numFmt numFmtId="201" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -2710,17 +2719,18 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2732,24 +2742,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2763,16 +2787,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2787,22 +2819,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2816,24 +2840,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2854,7 +2863,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2866,13 +2893,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2884,25 +2995,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2914,121 +3037,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3055,7 +3064,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3064,7 +3073,37 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3084,21 +3123,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -3106,21 +3130,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3144,124 +3153,124 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3270,16 +3279,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3618,19 +3627,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E818"/>
+  <dimension ref="A1:F818"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A795" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D736" sqref="D736"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="30.675" customWidth="1"/>
     <col min="2" max="2" width="22.95" customWidth="1"/>
+    <col min="4" max="4" width="45.95" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3646,6 +3656,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
@@ -11484,6 +11495,9 @@
       <c r="A712" s="1" t="s">
         <v>745</v>
       </c>
+      <c r="B712" s="1" t="s">
+        <v>746</v>
+      </c>
       <c r="C712" s="1" t="s">
         <v>6</v>
       </c>
@@ -11493,68 +11507,74 @@
     </row>
     <row r="713" spans="1:5">
       <c r="A713" s="1" t="s">
-        <v>746</v>
+        <v>747</v>
+      </c>
+      <c r="B713" s="1" t="s">
+        <v>748</v>
       </c>
       <c r="C713" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="E713" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="714" spans="1:5">
       <c r="A714" s="1" t="s">
-        <v>748</v>
+        <v>750</v>
+      </c>
+      <c r="B714" s="1" t="s">
+        <v>751</v>
       </c>
       <c r="C714" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="E714" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="715" spans="1:5">
       <c r="A715" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="C715" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="C715" s="1" t="s">
-        <v>747</v>
-      </c>
       <c r="E715" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="716" spans="1:5">
       <c r="A716" s="1" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="C716" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="E716" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="717" spans="1:5">
       <c r="A717" s="1" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
       <c r="C717" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="E717" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="718" spans="1:5">
       <c r="A718" s="1" t="s">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="C718" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="E718" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="719" spans="1:5">
@@ -11562,1158 +11582,1158 @@
         <v>245</v>
       </c>
       <c r="C719" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="E719" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="720" spans="1:5">
       <c r="A720" s="1" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="C720" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="E720" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="721" spans="1:5">
       <c r="A721" s="1" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="C721" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="E721" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="722" spans="1:5">
       <c r="A722" s="1" t="s">
-        <v>755</v>
+        <v>758</v>
       </c>
       <c r="C722" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="E722" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="723" spans="1:5">
       <c r="A723" s="1" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="C723" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="E723" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="724" spans="1:5">
       <c r="A724" s="1" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
       <c r="C724" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="E724" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="725" spans="1:5">
       <c r="A725" s="1" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="C725" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="E725" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="726" spans="1:5">
       <c r="A726" s="1" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="B726"/>
       <c r="C726" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="D726" s="1" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="E726" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="727" spans="1:5">
       <c r="A727" s="1" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
       <c r="C727" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="D727" s="1"/>
       <c r="E727" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="728" spans="1:5">
       <c r="A728" s="1" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="B728" s="1"/>
       <c r="C728" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E728" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="729" spans="1:5">
       <c r="A729" s="1" t="s">
-        <v>764</v>
+        <v>767</v>
       </c>
       <c r="B729" s="2"/>
       <c r="C729" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E729" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="730" spans="1:5">
       <c r="A730" s="1" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="B730"/>
       <c r="C730" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="D730" s="1"/>
       <c r="E730" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="731" spans="1:5">
       <c r="A731" s="1" t="s">
-        <v>766</v>
+        <v>769</v>
       </c>
       <c r="C731" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E731" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="732" spans="1:5">
       <c r="A732" s="1" t="s">
-        <v>767</v>
+        <v>770</v>
       </c>
       <c r="B732" s="1"/>
       <c r="C732" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E732" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="733" spans="1:5">
       <c r="A733" s="1" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="B733"/>
       <c r="C733" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="D733" s="1"/>
       <c r="E733" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="734" spans="1:5">
       <c r="A734" s="1" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
       <c r="B734" s="1"/>
       <c r="C734" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E734" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="735" spans="1:5">
       <c r="A735" s="1" t="s">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="C735" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E735" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="736" spans="1:5">
       <c r="A736" s="1" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="C736" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="D736" s="2" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="E736" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="737" spans="1:5">
       <c r="A737" s="1" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
       <c r="C737" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E737" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="738" spans="1:5">
       <c r="A738" s="1" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="C738" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E738" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="739" spans="1:5">
       <c r="A739" s="1" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
       <c r="C739" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E739" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="740" spans="1:5">
       <c r="A740" s="1" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="C740" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E740" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="741" spans="1:5">
       <c r="A741" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="C741" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="D741" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
       <c r="E741" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="742" spans="1:5">
       <c r="A742" s="1" t="s">
-        <v>779</v>
+        <v>782</v>
       </c>
       <c r="C742" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E742" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="743" spans="1:5">
       <c r="A743" s="1" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="C743" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E743" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="744" spans="1:5">
       <c r="A744" s="1" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="C744" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E744" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="745" spans="1:5">
       <c r="A745" s="1" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="C745" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E745" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="746" spans="1:5">
       <c r="A746" s="1" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c r="C746" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E746" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="747" spans="1:5">
       <c r="A747" s="1" t="s">
-        <v>784</v>
+        <v>787</v>
       </c>
       <c r="C747" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E747" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="748" spans="1:5">
       <c r="A748" s="1" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="C748" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E748" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="749" spans="1:5">
       <c r="A749" s="1" t="s">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="C749" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E749" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="750" spans="1:5">
       <c r="A750" s="1" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="C750" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E750" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="751" spans="1:5">
       <c r="A751" s="1" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="C751" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E751" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="752" spans="1:5">
       <c r="A752" s="1" t="s">
-        <v>789</v>
+        <v>792</v>
       </c>
       <c r="C752" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="D752" s="1" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
       <c r="E752" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="753" spans="1:5">
       <c r="A753" s="1" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c r="C753" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="D753" s="1" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="E753" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="754" spans="1:5">
       <c r="A754" s="1" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="C754" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="E754" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="755" spans="1:5">
       <c r="A755" s="1" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
       <c r="C755" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="D755" s="1" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="E755" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="756" spans="1:5">
       <c r="A756" s="1" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="C756" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="D756" s="1"/>
       <c r="E756" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="757" spans="1:5">
       <c r="A757" s="1" t="s">
-        <v>797</v>
+        <v>800</v>
       </c>
       <c r="C757" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="D757" s="1" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
       <c r="E757" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="758" spans="1:5">
       <c r="A758" s="1" t="s">
-        <v>799</v>
+        <v>802</v>
       </c>
       <c r="C758" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="E758" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="759" spans="1:5">
       <c r="A759" s="1" t="s">
-        <v>801</v>
+        <v>804</v>
       </c>
       <c r="C759" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="E759" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="760" spans="1:5">
       <c r="A760" s="1" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="C760" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="E760" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="761" spans="1:5">
       <c r="A761" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="C761" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="C761" s="1" t="s">
-        <v>800</v>
-      </c>
       <c r="E761" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="762" spans="1:5">
       <c r="A762" s="1" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c r="C762" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="E762" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="763" spans="1:5">
       <c r="A763" s="1" t="s">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="C763" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="E763" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="764" spans="1:5">
       <c r="A764" s="1" t="s">
-        <v>806</v>
+        <v>809</v>
       </c>
       <c r="C764" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="E764" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="765" spans="1:5">
       <c r="A765" s="1" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c r="C765" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="D765" s="1" t="s">
-        <v>808</v>
+        <v>811</v>
       </c>
       <c r="E765" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="766" spans="1:5">
       <c r="A766" s="1" t="s">
-        <v>809</v>
+        <v>812</v>
       </c>
       <c r="C766" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="E766" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="767" spans="1:5">
       <c r="A767" s="1" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="C767" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="E767" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="768" spans="1:5">
       <c r="A768" s="1" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
       <c r="C768" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="E768" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="769" spans="1:5">
       <c r="A769" s="1" t="s">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="C769" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E769" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="770" spans="1:5">
       <c r="A770" s="1" t="s">
-        <v>814</v>
+        <v>817</v>
       </c>
       <c r="C770" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E770" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="771" spans="1:5">
       <c r="A771" s="1" t="s">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c r="C771" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E771" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="772" spans="1:5">
       <c r="A772" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="C772" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="C772" s="1" t="s">
-        <v>813</v>
-      </c>
       <c r="E772" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="773" spans="1:5">
       <c r="A773" s="1" t="s">
-        <v>817</v>
+        <v>820</v>
       </c>
       <c r="C773" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E773" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="774" spans="1:5">
       <c r="A774" s="1" t="s">
-        <v>818</v>
+        <v>821</v>
       </c>
       <c r="C774" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E774" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="775" spans="1:5">
       <c r="A775" s="1" t="s">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="C775" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E775" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="776" spans="1:5">
       <c r="A776" s="1" t="s">
-        <v>820</v>
+        <v>823</v>
       </c>
       <c r="C776" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E776" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="777" spans="1:5">
       <c r="A777" s="1" t="s">
-        <v>821</v>
+        <v>824</v>
       </c>
       <c r="C777" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E777" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="778" spans="1:5">
       <c r="A778" s="1" t="s">
-        <v>822</v>
+        <v>825</v>
       </c>
       <c r="C778" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E778" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="779" spans="1:5">
       <c r="A779" s="1" t="s">
-        <v>823</v>
+        <v>826</v>
       </c>
       <c r="C779" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E779" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="780" spans="1:5">
       <c r="A780" s="1" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="C780" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E780" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="781" spans="1:5">
       <c r="A781" s="1" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="C781" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E781" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="782" spans="1:5">
       <c r="A782" s="1" t="s">
-        <v>826</v>
+        <v>829</v>
       </c>
       <c r="C782" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E782" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="783" spans="1:5">
       <c r="A783" s="1" t="s">
-        <v>827</v>
+        <v>830</v>
       </c>
       <c r="C783" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E783" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="784" spans="1:5">
       <c r="A784" s="1" t="s">
-        <v>828</v>
+        <v>831</v>
       </c>
       <c r="C784" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E784" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="785" spans="1:5">
       <c r="A785" s="1" t="s">
-        <v>829</v>
+        <v>832</v>
       </c>
       <c r="C785" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E785" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="786" spans="1:5">
       <c r="A786" s="1" t="s">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c r="C786" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E786" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="787" spans="1:5">
       <c r="A787" s="1" t="s">
-        <v>831</v>
+        <v>834</v>
       </c>
       <c r="C787" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E787" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="788" spans="1:5">
       <c r="A788" s="1" t="s">
-        <v>832</v>
+        <v>835</v>
       </c>
       <c r="C788" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E788" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="789" spans="1:5">
       <c r="A789" s="1" t="s">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c r="C789" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E789" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="790" spans="1:5">
       <c r="A790" s="1" t="s">
-        <v>834</v>
+        <v>837</v>
       </c>
       <c r="C790" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E790" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="791" spans="1:5">
       <c r="A791" s="1" t="s">
-        <v>835</v>
+        <v>838</v>
       </c>
       <c r="C791" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E791" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="792" spans="1:5">
       <c r="A792" s="1" t="s">
-        <v>836</v>
+        <v>839</v>
       </c>
       <c r="C792" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E792" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="793" spans="1:5">
       <c r="A793" s="1" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
       <c r="C793" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E793" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="794" spans="1:5">
       <c r="A794" s="1" t="s">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="C794" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E794" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="795" spans="1:5">
       <c r="A795" s="1" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c r="C795" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E795" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="796" spans="1:5">
       <c r="A796" s="1" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="C796" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E796" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="797" spans="1:5">
       <c r="A797" s="1" t="s">
-        <v>841</v>
+        <v>844</v>
       </c>
       <c r="C797" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E797" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="798" spans="1:5">
       <c r="A798" s="1" t="s">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c r="C798" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="D798" s="1" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c r="E798" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="799" spans="1:5">
       <c r="A799" s="1" t="s">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c r="C799" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E799" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="800" spans="1:5">
       <c r="A800" s="1" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
       <c r="C800" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E800" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="801" spans="1:5">
       <c r="A801" s="1" t="s">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c r="C801" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E801" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="802" spans="1:5">
       <c r="A802" s="1" t="s">
-        <v>847</v>
+        <v>850</v>
       </c>
       <c r="C802" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E802" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="803" spans="1:5">
       <c r="A803" s="1" t="s">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c r="C803" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="D803" s="1" t="s">
-        <v>849</v>
+        <v>852</v>
       </c>
       <c r="E803" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="804" spans="1:5">
       <c r="A804" s="1" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
       <c r="C804" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="D804" s="1" t="s">
-        <v>851</v>
+        <v>854</v>
       </c>
       <c r="E804" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="805" spans="1:5">
       <c r="A805" s="1" t="s">
-        <v>852</v>
+        <v>855</v>
       </c>
       <c r="C805" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E805" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="806" spans="1:5">
       <c r="A806" s="1" t="s">
-        <v>853</v>
+        <v>856</v>
       </c>
       <c r="C806" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E806" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="807" spans="1:5">
       <c r="A807" s="1" t="s">
-        <v>854</v>
+        <v>857</v>
       </c>
       <c r="C807" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E807" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="808" spans="1:5">
       <c r="A808" s="1" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="C808" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E808" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="809" spans="1:5">
       <c r="A809" s="1" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="C809" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E809" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="810" spans="1:5">
       <c r="A810" s="1" t="s">
-        <v>857</v>
+        <v>860</v>
       </c>
       <c r="C810" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="D810" s="1" t="s">
-        <v>858</v>
+        <v>861</v>
       </c>
       <c r="E810" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="811" spans="1:5">
       <c r="A811" s="1" t="s">
-        <v>859</v>
+        <v>862</v>
       </c>
       <c r="C811" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="D811" s="1" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
       <c r="E811" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="812" spans="1:5">
       <c r="A812" s="1" t="s">
-        <v>861</v>
+        <v>864</v>
       </c>
       <c r="C812" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="D812" s="1" t="s">
-        <v>862</v>
+        <v>865</v>
       </c>
       <c r="E812" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="813" spans="1:5">
       <c r="A813" s="1" t="s">
-        <v>863</v>
+        <v>866</v>
       </c>
       <c r="C813" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="D813" s="1" t="s">
-        <v>864</v>
+        <v>867</v>
       </c>
       <c r="E813" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="814" spans="1:5">
       <c r="A814" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="C814" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E814" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="815" spans="1:5">
       <c r="A815" s="1" t="s">
-        <v>866</v>
+        <v>869</v>
       </c>
       <c r="C815" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E815" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="816" spans="1:5">
       <c r="A816" s="1" t="s">
-        <v>867</v>
+        <v>870</v>
       </c>
       <c r="C816" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E816" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="817" spans="1:5">
       <c r="A817" s="1" t="s">
-        <v>868</v>
+        <v>871</v>
       </c>
       <c r="C817" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E817" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="818" spans="1:5">
       <c r="A818" s="1" t="s">
-        <v>869</v>
+        <v>872</v>
       </c>
       <c r="C818" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="D818" s="1" t="s">
-        <v>870</v>
+        <v>873</v>
       </c>
       <c r="E818" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated song list 2022/4/17
</commit_message>
<xml_diff>
--- a/music_list_7.xlsx
+++ b/music_list_7.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1008</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1023</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4586" uniqueCount="1798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4600" uniqueCount="1804">
   <si>
     <t>歌名</t>
   </si>
@@ -4634,6 +4634,12 @@
     <t>アンコール/安可</t>
   </si>
   <si>
+    <t>怪物</t>
+  </si>
+  <si>
+    <t>《动物狂想曲》第一季OP</t>
+  </si>
+  <si>
     <t>My Friend(マイフレンド)</t>
   </si>
   <si>
@@ -4656,6 +4662,15 @@
   </si>
   <si>
     <t>煙</t>
+  </si>
+  <si>
+    <t>いけないボーダーライン/禁忌的边界线</t>
+  </si>
+  <si>
+    <t>ワルキューレ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">《超时空要塞Δ》插曲 </t>
   </si>
   <si>
     <t>iB.</t>
@@ -5389,6 +5404,9 @@
     <t>威猛乐队</t>
   </si>
   <si>
+    <t>Rubia</t>
+  </si>
+  <si>
     <t>粤语</t>
   </si>
   <si>
@@ -5475,44 +5493,44 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="39">
-    <numFmt numFmtId="176" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
+    <numFmt numFmtId="176" formatCode="#\ ??/??"/>
+    <numFmt numFmtId="177" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="178" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="179" formatCode="m/d"/>
+    <numFmt numFmtId="180" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="181" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
+    <numFmt numFmtId="182" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
+    <numFmt numFmtId="183" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="184" formatCode="#\ ?/?"/>
     <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="185" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="186" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="187" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="188" formatCode="yy/m/d"/>
     <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="179" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="180" formatCode="[$-804]aaa"/>
-    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="181" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="182" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="183" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="189" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="190" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="184" formatCode="mmmmm"/>
-    <numFmt numFmtId="185" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="186" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="187" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="188" formatCode="#\ ??/??"/>
-    <numFmt numFmtId="189" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="190" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="191" formatCode="yy/m/d"/>
-    <numFmt numFmtId="192" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="193" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="194" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="195" formatCode="mmmm\-yy"/>
-    <numFmt numFmtId="196" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="197" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
+    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="191" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="192" formatCode="mmmmm\-yy"/>
+    <numFmt numFmtId="193" formatCode="mmmmm"/>
+    <numFmt numFmtId="194" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="195" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="196" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="197" formatCode="\¥#,##0;\¥\-#,##0"/>
     <numFmt numFmtId="198" formatCode="#\ ??"/>
-    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
-    <numFmt numFmtId="199" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="200" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="201" formatCode="m/d"/>
+    <numFmt numFmtId="199" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
+    <numFmt numFmtId="200" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+    <numFmt numFmtId="201" formatCode="mmmm\-yy"/>
     <numFmt numFmtId="202" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="44">
@@ -5676,18 +5694,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -5708,24 +5733,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -5737,9 +5747,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5754,7 +5801,15 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -5763,36 +5818,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5800,14 +5826,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5841,169 +5859,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6021,7 +5883,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6062,17 +6080,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -6084,6 +6091,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6137,76 +6155,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="196" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -6215,81 +6233,81 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="202" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="197" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -6304,10 +6322,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="197" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="197" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="199" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
@@ -6345,18 +6363,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="197" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="197" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -6707,12 +6713,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G1020"/>
+  <dimension ref="A1:G1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1014" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1011" sqref="A1011"/>
+      <selection pane="bottomLeft" activeCell="B1021" sqref="B1021"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -7634,7 +7640,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -20807,46 +20813,46 @@
       </c>
     </row>
     <row r="638" spans="1:7">
-      <c r="A638" s="21" t="s">
+      <c r="A638" s="4" t="s">
         <v>1092</v>
       </c>
-      <c r="B638" s="21" t="s">
+      <c r="B638" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="C638" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D638" s="22"/>
-      <c r="E638" s="21" t="s">
+      <c r="C638" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D638" s="5"/>
+      <c r="E638" s="4" t="s">
         <v>1043</v>
       </c>
-      <c r="F638" s="23">
-        <v>0</v>
-      </c>
-      <c r="G638" s="23">
+      <c r="F638" s="7">
+        <v>0</v>
+      </c>
+      <c r="G638" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="639" spans="1:7">
-      <c r="A639" s="21" t="s">
+      <c r="A639" s="4" t="s">
         <v>1093</v>
       </c>
-      <c r="B639" s="21" t="s">
+      <c r="B639" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="C639" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D639" s="21" t="s">
+      <c r="C639" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D639" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E639" s="21" t="s">
+      <c r="E639" s="4" t="s">
         <v>1043</v>
       </c>
-      <c r="F639" s="24">
-        <v>0</v>
-      </c>
-      <c r="G639" s="23">
+      <c r="F639" s="8">
+        <v>0</v>
+      </c>
+      <c r="G639" s="7">
         <v>0</v>
       </c>
     </row>
@@ -21732,7 +21738,7 @@
       <c r="A680" s="5" t="s">
         <v>1152</v>
       </c>
-      <c r="B680" s="25" t="s">
+      <c r="B680" s="21" t="s">
         <v>1153</v>
       </c>
       <c r="C680" s="4" t="s">
@@ -23744,23 +23750,23 @@
       </c>
     </row>
     <row r="773" spans="1:7">
-      <c r="A773" s="21" t="s">
+      <c r="A773" s="4" t="s">
         <v>1304</v>
       </c>
-      <c r="B773" s="21" t="s">
+      <c r="B773" s="4" t="s">
         <v>1305</v>
       </c>
-      <c r="C773" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D773" s="22"/>
-      <c r="E773" s="21" t="s">
+      <c r="C773" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D773" s="5"/>
+      <c r="E773" s="4" t="s">
         <v>1222</v>
       </c>
-      <c r="F773" s="24">
-        <v>0</v>
-      </c>
-      <c r="G773" s="23">
+      <c r="F773" s="8">
+        <v>0</v>
+      </c>
+      <c r="G773" s="7">
         <v>0</v>
       </c>
     </row>
@@ -25529,7 +25535,7 @@
       <c r="C855" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D855" s="26" t="s">
+      <c r="D855" s="22" t="s">
         <v>1441</v>
       </c>
       <c r="E855" s="4" t="s">
@@ -25774,7 +25780,7 @@
       <c r="C866" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D866" s="27" t="s">
+      <c r="D866" s="23" t="s">
         <v>1463</v>
       </c>
       <c r="E866" s="4" t="s">
@@ -25877,13 +25883,13 @@
       <c r="A871" s="4" t="s">
         <v>1473</v>
       </c>
-      <c r="B871" s="27" t="s">
+      <c r="B871" s="23" t="s">
         <v>1474</v>
       </c>
       <c r="C871" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D871" s="27" t="s">
+      <c r="D871" s="23" t="s">
         <v>1475</v>
       </c>
       <c r="E871" s="4" t="s">
@@ -25943,16 +25949,16 @@
       </c>
     </row>
     <row r="874" ht="14.25" spans="1:7">
-      <c r="A874" s="28" t="s">
+      <c r="A874" s="24" t="s">
         <v>1482</v>
       </c>
-      <c r="B874" s="28" t="s">
+      <c r="B874" s="24" t="s">
         <v>1483</v>
       </c>
       <c r="C874" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D874" s="29" t="s">
+      <c r="D874" s="25" t="s">
         <v>1484</v>
       </c>
       <c r="E874" s="4" t="s">
@@ -25996,7 +26002,7 @@
       <c r="C876" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D876" s="27" t="s">
+      <c r="D876" s="23" t="s">
         <v>1489</v>
       </c>
       <c r="E876" s="4" t="s">
@@ -26287,7 +26293,7 @@
       <c r="C889" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D889" s="27" t="s">
+      <c r="D889" s="23" t="s">
         <v>1521</v>
       </c>
       <c r="E889" s="4" t="s">
@@ -26430,20 +26436,20 @@
       <c r="A896" s="4" t="s">
         <v>1529</v>
       </c>
-      <c r="B896" s="5" t="s">
+      <c r="B896" s="4" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C896" s="4" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D896" s="4" t="s">
         <v>1530</v>
       </c>
-      <c r="C896" s="5" t="s">
+      <c r="E896" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D896" s="4" t="s">
-        <v>1531</v>
-      </c>
-      <c r="E896" s="5" t="s">
-        <v>1440</v>
-      </c>
       <c r="F896" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G896" s="7">
         <v>0</v>
@@ -26451,18 +26457,18 @@
     </row>
     <row r="897" spans="1:7">
       <c r="A897" s="4" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B897" s="5" t="s">
         <v>1532</v>
       </c>
-      <c r="B897" s="5" t="s">
+      <c r="C897" s="5" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D897" s="4" t="s">
         <v>1533</v>
       </c>
-      <c r="C897" s="4" t="s">
-        <v>1440</v>
-      </c>
-      <c r="D897" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E897" s="4" t="s">
+      <c r="E897" s="5" t="s">
         <v>1440</v>
       </c>
       <c r="F897" s="7">
@@ -26483,7 +26489,7 @@
         <v>1440</v>
       </c>
       <c r="D898" s="4" t="s">
-        <v>1536</v>
+        <v>14</v>
       </c>
       <c r="E898" s="4" t="s">
         <v>1440</v>
@@ -26495,17 +26501,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="899" ht="14.25" spans="1:7">
-      <c r="A899" s="5" t="s">
+    <row r="899" spans="1:7">
+      <c r="A899" s="4" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B899" s="5" t="s">
         <v>1537</v>
-      </c>
-      <c r="B899" s="30" t="s">
-        <v>1538</v>
       </c>
       <c r="C899" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D899" s="5"/>
+      <c r="D899" s="4" t="s">
+        <v>1538</v>
+      </c>
       <c r="E899" s="4" t="s">
         <v>1440</v>
       </c>
@@ -26526,24 +26534,24 @@
       <c r="C900" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D900" s="4" t="s">
+      <c r="D900" s="5" t="s">
         <v>1541</v>
       </c>
       <c r="E900" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F900" s="8">
+      <c r="F900" s="7">
         <v>0</v>
       </c>
       <c r="G900" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="901" spans="1:7">
-      <c r="A901" s="4" t="s">
+    <row r="901" ht="14.25" spans="1:7">
+      <c r="A901" s="5" t="s">
         <v>1542</v>
       </c>
-      <c r="B901" s="4" t="s">
+      <c r="B901" s="26" t="s">
         <v>1543</v>
       </c>
       <c r="C901" s="4" t="s">
@@ -26561,7 +26569,7 @@
       </c>
     </row>
     <row r="902" spans="1:7">
-      <c r="A902" s="5" t="s">
+      <c r="A902" s="4" t="s">
         <v>1544</v>
       </c>
       <c r="B902" s="4" t="s">
@@ -26576,7 +26584,7 @@
       <c r="E902" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F902" s="7">
+      <c r="F902" s="8">
         <v>0</v>
       </c>
       <c r="G902" s="7">
@@ -26584,7 +26592,7 @@
       </c>
     </row>
     <row r="903" spans="1:7">
-      <c r="A903" s="5" t="s">
+      <c r="A903" s="4" t="s">
         <v>1547</v>
       </c>
       <c r="B903" s="4" t="s">
@@ -26597,7 +26605,7 @@
       <c r="E903" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F903" s="8">
+      <c r="F903" s="7">
         <v>0</v>
       </c>
       <c r="G903" s="7">
@@ -26608,7 +26616,7 @@
       <c r="A904" s="5" t="s">
         <v>1549</v>
       </c>
-      <c r="B904" s="5" t="s">
+      <c r="B904" s="4" t="s">
         <v>1550</v>
       </c>
       <c r="C904" s="4" t="s">
@@ -26628,7 +26636,7 @@
       </c>
     </row>
     <row r="905" spans="1:7">
-      <c r="A905" s="4" t="s">
+      <c r="A905" s="5" t="s">
         <v>1552</v>
       </c>
       <c r="B905" s="4" t="s">
@@ -26641,7 +26649,7 @@
       <c r="E905" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F905" s="7">
+      <c r="F905" s="8">
         <v>0</v>
       </c>
       <c r="G905" s="7">
@@ -26649,16 +26657,18 @@
       </c>
     </row>
     <row r="906" spans="1:7">
-      <c r="A906" s="28" t="s">
+      <c r="A906" s="5" t="s">
         <v>1554</v>
       </c>
-      <c r="B906" s="4" t="s">
+      <c r="B906" s="5" t="s">
         <v>1555</v>
       </c>
       <c r="C906" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D906" s="5"/>
+      <c r="D906" s="4" t="s">
+        <v>1556</v>
+      </c>
       <c r="E906" s="4" t="s">
         <v>1440</v>
       </c>
@@ -26670,11 +26680,11 @@
       </c>
     </row>
     <row r="907" spans="1:7">
-      <c r="A907" s="5" t="s">
-        <v>1556</v>
+      <c r="A907" s="4" t="s">
+        <v>1557</v>
       </c>
       <c r="B907" s="4" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
       <c r="C907" s="4" t="s">
         <v>1440</v>
@@ -26691,18 +26701,16 @@
       </c>
     </row>
     <row r="908" spans="1:7">
-      <c r="A908" s="4" t="s">
-        <v>1557</v>
+      <c r="A908" s="24" t="s">
+        <v>1559</v>
       </c>
       <c r="B908" s="4" t="s">
-        <v>1555</v>
+        <v>1560</v>
       </c>
       <c r="C908" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D908" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="D908" s="5"/>
       <c r="E908" s="4" t="s">
         <v>1440</v>
       </c>
@@ -26714,11 +26722,11 @@
       </c>
     </row>
     <row r="909" spans="1:7">
-      <c r="A909" s="4" t="s">
-        <v>1558</v>
+      <c r="A909" s="5" t="s">
+        <v>1561</v>
       </c>
       <c r="B909" s="4" t="s">
-        <v>1555</v>
+        <v>1560</v>
       </c>
       <c r="C909" s="4" t="s">
         <v>1440</v>
@@ -26735,8 +26743,8 @@
       </c>
     </row>
     <row r="910" spans="1:7">
-      <c r="A910" s="5" t="s">
-        <v>1559</v>
+      <c r="A910" s="4" t="s">
+        <v>1562</v>
       </c>
       <c r="B910" s="4" t="s">
         <v>1560</v>
@@ -26745,7 +26753,7 @@
         <v>1440</v>
       </c>
       <c r="D910" s="4" t="s">
-        <v>1561</v>
+        <v>14</v>
       </c>
       <c r="E910" s="4" t="s">
         <v>1440</v>
@@ -26759,7 +26767,7 @@
     </row>
     <row r="911" spans="1:7">
       <c r="A911" s="4" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="B911" s="4" t="s">
         <v>1560</v>
@@ -26767,9 +26775,7 @@
       <c r="C911" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D911" s="4" t="s">
-        <v>1563</v>
-      </c>
+      <c r="D911" s="5"/>
       <c r="E911" s="4" t="s">
         <v>1440</v>
       </c>
@@ -26781,17 +26787,17 @@
       </c>
     </row>
     <row r="912" spans="1:7">
-      <c r="A912" s="4" t="s">
+      <c r="A912" s="5" t="s">
         <v>1564</v>
       </c>
       <c r="B912" s="4" t="s">
-        <v>1560</v>
+        <v>1565</v>
       </c>
       <c r="C912" s="4" t="s">
         <v>1440</v>
       </c>
       <c r="D912" s="4" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="E912" s="4" t="s">
         <v>1440</v>
@@ -26805,19 +26811,21 @@
     </row>
     <row r="913" spans="1:7">
       <c r="A913" s="4" t="s">
-        <v>1566</v>
-      </c>
-      <c r="B913" s="5" t="s">
         <v>1567</v>
+      </c>
+      <c r="B913" s="4" t="s">
+        <v>1565</v>
       </c>
       <c r="C913" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D913" s="5"/>
+      <c r="D913" s="4" t="s">
+        <v>1568</v>
+      </c>
       <c r="E913" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F913" s="8">
+      <c r="F913" s="7">
         <v>0</v>
       </c>
       <c r="G913" s="7">
@@ -26826,10 +26834,10 @@
     </row>
     <row r="914" spans="1:7">
       <c r="A914" s="4" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="B914" s="4" t="s">
-        <v>1569</v>
+        <v>1565</v>
       </c>
       <c r="C914" s="4" t="s">
         <v>1440</v>
@@ -26851,19 +26859,17 @@
       <c r="A915" s="4" t="s">
         <v>1571</v>
       </c>
-      <c r="B915" s="4" t="s">
+      <c r="B915" s="5" t="s">
         <v>1572</v>
       </c>
       <c r="C915" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D915" s="4" t="s">
-        <v>1573</v>
-      </c>
+      <c r="D915" s="5"/>
       <c r="E915" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F915" s="7">
+      <c r="F915" s="8">
         <v>0</v>
       </c>
       <c r="G915" s="7">
@@ -26872,18 +26878,18 @@
     </row>
     <row r="916" spans="1:7">
       <c r="A916" s="4" t="s">
+        <v>1573</v>
+      </c>
+      <c r="B916" s="4" t="s">
         <v>1574</v>
       </c>
-      <c r="B916" s="5" t="s">
+      <c r="C916" s="4" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D916" s="4" t="s">
         <v>1575</v>
       </c>
-      <c r="C916" s="5" t="s">
-        <v>1440</v>
-      </c>
-      <c r="D916" s="5" t="s">
-        <v>1576</v>
-      </c>
-      <c r="E916" s="5" t="s">
+      <c r="E916" s="4" t="s">
         <v>1440</v>
       </c>
       <c r="F916" s="7">
@@ -26895,21 +26901,21 @@
     </row>
     <row r="917" spans="1:7">
       <c r="A917" s="4" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B917" s="4" t="s">
         <v>1577</v>
-      </c>
-      <c r="B917" s="31" t="s">
-        <v>1578</v>
       </c>
       <c r="C917" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D917" s="5" t="s">
-        <v>1579</v>
+      <c r="D917" s="4" t="s">
+        <v>1578</v>
       </c>
       <c r="E917" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F917" s="8">
+      <c r="F917" s="7">
         <v>0</v>
       </c>
       <c r="G917" s="7">
@@ -26918,18 +26924,18 @@
     </row>
     <row r="918" spans="1:7">
       <c r="A918" s="4" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B918" s="5" t="s">
         <v>1580</v>
       </c>
-      <c r="B918" s="4" t="s">
+      <c r="C918" s="5" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D918" s="5" t="s">
         <v>1581</v>
       </c>
-      <c r="C918" s="4" t="s">
-        <v>1440</v>
-      </c>
-      <c r="D918" s="6" t="s">
-        <v>1582</v>
-      </c>
-      <c r="E918" s="4" t="s">
+      <c r="E918" s="5" t="s">
         <v>1440</v>
       </c>
       <c r="F918" s="7">
@@ -26941,44 +26947,44 @@
     </row>
     <row r="919" spans="1:7">
       <c r="A919" s="4" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B919" s="27" t="s">
         <v>1583</v>
-      </c>
-      <c r="B919" s="4" t="s">
-        <v>1584</v>
       </c>
       <c r="C919" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D919" s="4" t="s">
-        <v>1585</v>
+      <c r="D919" s="5" t="s">
+        <v>1584</v>
       </c>
       <c r="E919" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F919" s="7">
+      <c r="F919" s="8">
         <v>0</v>
       </c>
       <c r="G919" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="920" spans="1:7">
       <c r="A920" s="4" t="s">
+        <v>1585</v>
+      </c>
+      <c r="B920" s="4" t="s">
         <v>1586</v>
-      </c>
-      <c r="B920" s="14" t="s">
-        <v>1587</v>
       </c>
       <c r="C920" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D920" s="4" t="s">
-        <v>1588</v>
+      <c r="D920" s="6" t="s">
+        <v>1587</v>
       </c>
       <c r="E920" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F920" s="8">
+      <c r="F920" s="7">
         <v>0</v>
       </c>
       <c r="G920" s="7">
@@ -26986,31 +26992,33 @@
       </c>
     </row>
     <row r="921" spans="1:7">
-      <c r="A921" s="5" t="s">
+      <c r="A921" s="4" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B921" s="4" t="s">
         <v>1589</v>
-      </c>
-      <c r="B921" s="5" t="s">
-        <v>1590</v>
       </c>
       <c r="C921" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D921" s="5"/>
+      <c r="D921" s="4" t="s">
+        <v>1590</v>
+      </c>
       <c r="E921" s="4" t="s">
         <v>1440</v>
       </c>
       <c r="F921" s="7">
+        <v>0</v>
+      </c>
+      <c r="G921" s="7">
         <v>1</v>
       </c>
-      <c r="G921" s="7">
-        <v>0</v>
-      </c>
     </row>
     <row r="922" spans="1:7">
-      <c r="A922" s="5" t="s">
+      <c r="A922" s="4" t="s">
         <v>1591</v>
       </c>
-      <c r="B922" s="4" t="s">
+      <c r="B922" s="14" t="s">
         <v>1592</v>
       </c>
       <c r="C922" s="4" t="s">
@@ -27030,39 +27038,39 @@
       </c>
     </row>
     <row r="923" spans="1:7">
-      <c r="A923" s="4" t="s">
+      <c r="A923" s="5" t="s">
         <v>1594</v>
       </c>
-      <c r="B923" s="4" t="s">
+      <c r="B923" s="5" t="s">
         <v>1595</v>
       </c>
       <c r="C923" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D923" s="4" t="s">
-        <v>1596</v>
-      </c>
+      <c r="D923" s="5"/>
       <c r="E923" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F923" s="8">
-        <v>0</v>
+      <c r="F923" s="7">
+        <v>1</v>
       </c>
       <c r="G923" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="924" spans="1:7">
-      <c r="A924" s="4" t="s">
+      <c r="A924" s="5" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B924" s="4" t="s">
         <v>1597</v>
-      </c>
-      <c r="B924" s="5" t="s">
-        <v>1598</v>
       </c>
       <c r="C924" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D924" s="5"/>
+      <c r="D924" s="4" t="s">
+        <v>1598</v>
+      </c>
       <c r="E924" s="4" t="s">
         <v>1440</v>
       </c>
@@ -27083,7 +27091,9 @@
       <c r="C925" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D925" s="5"/>
+      <c r="D925" s="4" t="s">
+        <v>1601</v>
+      </c>
       <c r="E925" s="4" t="s">
         <v>1440</v>
       </c>
@@ -27096,10 +27106,10 @@
     </row>
     <row r="926" spans="1:7">
       <c r="A926" s="4" t="s">
-        <v>1601</v>
-      </c>
-      <c r="B926" s="4" t="s">
-        <v>1600</v>
+        <v>1602</v>
+      </c>
+      <c r="B926" s="5" t="s">
+        <v>1603</v>
       </c>
       <c r="C926" s="4" t="s">
         <v>1440</v>
@@ -27108,7 +27118,7 @@
       <c r="E926" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F926" s="7">
+      <c r="F926" s="8">
         <v>0</v>
       </c>
       <c r="G926" s="7">
@@ -27116,22 +27126,20 @@
       </c>
     </row>
     <row r="927" spans="1:7">
-      <c r="A927" s="5" t="s">
-        <v>1602</v>
+      <c r="A927" s="4" t="s">
+        <v>1604</v>
       </c>
       <c r="B927" s="4" t="s">
-        <v>1603</v>
+        <v>1605</v>
       </c>
       <c r="C927" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D927" s="4" t="s">
-        <v>1604</v>
-      </c>
+      <c r="D927" s="5"/>
       <c r="E927" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F927" s="7">
+      <c r="F927" s="8">
         <v>0</v>
       </c>
       <c r="G927" s="7">
@@ -27140,42 +27148,42 @@
     </row>
     <row r="928" spans="1:7">
       <c r="A928" s="4" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B928" s="4" t="s">
         <v>1605</v>
       </c>
-      <c r="B928" s="5" t="s">
-        <v>1606</v>
-      </c>
-      <c r="C928" s="5" t="s">
+      <c r="C928" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D928" s="5" t="s">
+      <c r="D928" s="5"/>
+      <c r="E928" s="4" t="s">
+        <v>1440</v>
+      </c>
+      <c r="F928" s="7">
+        <v>0</v>
+      </c>
+      <c r="G928" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="929" spans="1:7">
+      <c r="A929" s="5" t="s">
         <v>1607</v>
       </c>
-      <c r="E928" s="5" t="s">
-        <v>1440</v>
-      </c>
-      <c r="F928" s="7">
-        <v>0</v>
-      </c>
-      <c r="G928" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="929" spans="1:7">
-      <c r="A929" s="4" t="s">
+      <c r="B929" s="4" t="s">
         <v>1608</v>
-      </c>
-      <c r="B929" s="5" t="s">
-        <v>1609</v>
       </c>
       <c r="C929" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D929" s="5"/>
+      <c r="D929" s="4" t="s">
+        <v>1609</v>
+      </c>
       <c r="E929" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F929" s="8">
+      <c r="F929" s="7">
         <v>0</v>
       </c>
       <c r="G929" s="7">
@@ -27183,19 +27191,19 @@
       </c>
     </row>
     <row r="930" spans="1:7">
-      <c r="A930" s="5" t="s">
+      <c r="A930" s="4" t="s">
         <v>1610</v>
       </c>
-      <c r="B930" s="4" t="s">
+      <c r="B930" s="5" t="s">
         <v>1611</v>
       </c>
-      <c r="C930" s="4" t="s">
+      <c r="C930" s="5" t="s">
         <v>1440</v>
       </c>
-      <c r="D930" s="4" t="s">
+      <c r="D930" s="5" t="s">
         <v>1612</v>
       </c>
-      <c r="E930" s="4" t="s">
+      <c r="E930" s="5" t="s">
         <v>1440</v>
       </c>
       <c r="F930" s="7">
@@ -27209,19 +27217,17 @@
       <c r="A931" s="4" t="s">
         <v>1613</v>
       </c>
-      <c r="B931" s="4" t="s">
+      <c r="B931" s="5" t="s">
         <v>1614</v>
       </c>
       <c r="C931" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D931" s="4" t="s">
-        <v>1615</v>
-      </c>
+      <c r="D931" s="5"/>
       <c r="E931" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F931" s="7">
+      <c r="F931" s="8">
         <v>0</v>
       </c>
       <c r="G931" s="7">
@@ -27229,22 +27235,22 @@
       </c>
     </row>
     <row r="932" spans="1:7">
-      <c r="A932" s="4" t="s">
+      <c r="A932" s="5" t="s">
+        <v>1615</v>
+      </c>
+      <c r="B932" s="4" t="s">
         <v>1616</v>
-      </c>
-      <c r="B932" s="5" t="s">
-        <v>1617</v>
       </c>
       <c r="C932" s="4" t="s">
         <v>1440</v>
       </c>
       <c r="D932" s="4" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="E932" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F932" s="8">
+      <c r="F932" s="7">
         <v>0</v>
       </c>
       <c r="G932" s="7">
@@ -27253,15 +27259,17 @@
     </row>
     <row r="933" spans="1:7">
       <c r="A933" s="4" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B933" s="4" t="s">
         <v>1619</v>
-      </c>
-      <c r="B933" s="5" t="s">
-        <v>1620</v>
       </c>
       <c r="C933" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D933" s="5"/>
+      <c r="D933" s="4" t="s">
+        <v>1620</v>
+      </c>
       <c r="E933" s="4" t="s">
         <v>1440</v>
       </c>
@@ -27276,17 +27284,19 @@
       <c r="A934" s="4" t="s">
         <v>1621</v>
       </c>
-      <c r="B934" s="4" t="s">
+      <c r="B934" s="5" t="s">
         <v>1622</v>
       </c>
       <c r="C934" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D934" s="5"/>
+      <c r="D934" s="4" t="s">
+        <v>1623</v>
+      </c>
       <c r="E934" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F934" s="7">
+      <c r="F934" s="8">
         <v>0</v>
       </c>
       <c r="G934" s="7">
@@ -27295,17 +27305,15 @@
     </row>
     <row r="935" spans="1:7">
       <c r="A935" s="4" t="s">
-        <v>1623</v>
-      </c>
-      <c r="B935" s="4" t="s">
-        <v>1622</v>
+        <v>1624</v>
+      </c>
+      <c r="B935" s="5" t="s">
+        <v>1625</v>
       </c>
       <c r="C935" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D935" s="4" t="s">
-        <v>1624</v>
-      </c>
+      <c r="D935" s="5"/>
       <c r="E935" s="4" t="s">
         <v>1440</v>
       </c>
@@ -27318,21 +27326,19 @@
     </row>
     <row r="936" spans="1:7">
       <c r="A936" s="4" t="s">
-        <v>1625</v>
+        <v>1626</v>
       </c>
       <c r="B936" s="4" t="s">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="C936" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D936" s="4" t="s">
-        <v>1627</v>
-      </c>
+      <c r="D936" s="5"/>
       <c r="E936" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F936" s="8">
+      <c r="F936" s="7">
         <v>0</v>
       </c>
       <c r="G936" s="7">
@@ -27340,17 +27346,17 @@
       </c>
     </row>
     <row r="937" spans="1:7">
-      <c r="A937" s="5" t="s">
+      <c r="A937" s="4" t="s">
         <v>1628</v>
       </c>
-      <c r="B937" s="26" t="s">
-        <v>1629</v>
+      <c r="B937" s="4" t="s">
+        <v>1627</v>
       </c>
       <c r="C937" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D937" s="27" t="s">
-        <v>1630</v>
+      <c r="D937" s="4" t="s">
+        <v>1629</v>
       </c>
       <c r="E937" s="4" t="s">
         <v>1440</v>
@@ -27364,15 +27370,17 @@
     </row>
     <row r="938" spans="1:7">
       <c r="A938" s="4" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B938" s="4" t="s">
         <v>1631</v>
-      </c>
-      <c r="B938" s="4" t="s">
-        <v>1632</v>
       </c>
       <c r="C938" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D938" s="5"/>
+      <c r="D938" s="4" t="s">
+        <v>1632</v>
+      </c>
       <c r="E938" s="4" t="s">
         <v>1440</v>
       </c>
@@ -27384,22 +27392,22 @@
       </c>
     </row>
     <row r="939" spans="1:7">
-      <c r="A939" s="4" t="s">
+      <c r="A939" s="5" t="s">
         <v>1633</v>
       </c>
-      <c r="B939" s="4" t="s">
-        <v>1632</v>
+      <c r="B939" s="22" t="s">
+        <v>1634</v>
       </c>
       <c r="C939" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D939" s="4" t="s">
-        <v>1634</v>
+      <c r="D939" s="23" t="s">
+        <v>1635</v>
       </c>
       <c r="E939" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F939" s="8">
+      <c r="F939" s="7">
         <v>0</v>
       </c>
       <c r="G939" s="7">
@@ -27408,21 +27416,19 @@
     </row>
     <row r="940" spans="1:7">
       <c r="A940" s="4" t="s">
-        <v>1635</v>
+        <v>1636</v>
       </c>
       <c r="B940" s="4" t="s">
-        <v>1636</v>
+        <v>1637</v>
       </c>
       <c r="C940" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D940" s="4" t="s">
-        <v>1612</v>
-      </c>
+      <c r="D940" s="5"/>
       <c r="E940" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F940" s="7">
+      <c r="F940" s="8">
         <v>0</v>
       </c>
       <c r="G940" s="7">
@@ -27431,10 +27437,10 @@
     </row>
     <row r="941" spans="1:7">
       <c r="A941" s="4" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B941" s="4" t="s">
         <v>1637</v>
-      </c>
-      <c r="B941" s="4" t="s">
-        <v>1638</v>
       </c>
       <c r="C941" s="4" t="s">
         <v>1440</v>
@@ -27445,7 +27451,7 @@
       <c r="E941" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="F941" s="7">
+      <c r="F941" s="8">
         <v>0</v>
       </c>
       <c r="G941" s="7">
@@ -27453,17 +27459,19 @@
       </c>
     </row>
     <row r="942" spans="1:7">
-      <c r="A942" s="5" t="s">
+      <c r="A942" s="4" t="s">
         <v>1640</v>
       </c>
-      <c r="B942" s="5" t="s">
-        <v>1638</v>
-      </c>
-      <c r="C942" s="5" t="s">
+      <c r="B942" s="4" t="s">
+        <v>1641</v>
+      </c>
+      <c r="C942" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D942" s="5"/>
-      <c r="E942" s="5" t="s">
+      <c r="D942" s="4" t="s">
+        <v>1617</v>
+      </c>
+      <c r="E942" s="4" t="s">
         <v>1440</v>
       </c>
       <c r="F942" s="7">
@@ -27475,16 +27483,16 @@
     </row>
     <row r="943" spans="1:7">
       <c r="A943" s="4" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="B943" s="4" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="C943" s="4" t="s">
         <v>1440</v>
       </c>
       <c r="D943" s="4" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="E943" s="4" t="s">
         <v>1440</v>
@@ -27497,17 +27505,17 @@
       </c>
     </row>
     <row r="944" spans="1:7">
-      <c r="A944" s="4" t="s">
-        <v>1644</v>
+      <c r="A944" s="5" t="s">
+        <v>1645</v>
       </c>
       <c r="B944" s="5" t="s">
-        <v>1645</v>
-      </c>
-      <c r="C944" s="4" t="s">
+        <v>1643</v>
+      </c>
+      <c r="C944" s="5" t="s">
         <v>1440</v>
       </c>
       <c r="D944" s="5"/>
-      <c r="E944" s="4" t="s">
+      <c r="E944" s="5" t="s">
         <v>1440</v>
       </c>
       <c r="F944" s="7">
@@ -27527,7 +27535,7 @@
       <c r="C945" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="D945" s="27" t="s">
+      <c r="D945" s="4" t="s">
         <v>1648</v>
       </c>
       <c r="E945" s="4" t="s">
@@ -27545,13 +27553,13 @@
         <v>1649</v>
       </c>
       <c r="B946" s="5" t="s">
-        <v>1647</v>
-      </c>
-      <c r="C946" s="5" t="s">
+        <v>1650</v>
+      </c>
+      <c r="C946" s="4" t="s">
         <v>1440</v>
       </c>
       <c r="D946" s="5"/>
-      <c r="E946" s="5" t="s">
+      <c r="E946" s="4" t="s">
         <v>1440</v>
       </c>
       <c r="F946" s="7">
@@ -27563,17 +27571,19 @@
     </row>
     <row r="947" spans="1:7">
       <c r="A947" s="4" t="s">
-        <v>1650</v>
-      </c>
-      <c r="B947" s="5" t="s">
         <v>1651</v>
       </c>
+      <c r="B947" s="4" t="s">
+        <v>1652</v>
+      </c>
       <c r="C947" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D947" s="5"/>
+        <v>1440</v>
+      </c>
+      <c r="D947" s="23" t="s">
+        <v>1653</v>
+      </c>
       <c r="E947" s="4" t="s">
-        <v>1652</v>
+        <v>1440</v>
       </c>
       <c r="F947" s="7">
         <v>0</v>
@@ -27584,19 +27594,17 @@
     </row>
     <row r="948" spans="1:7">
       <c r="A948" s="4" t="s">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="B948" s="5" t="s">
-        <v>1654</v>
-      </c>
-      <c r="C948" s="4" t="s">
         <v>1652</v>
       </c>
-      <c r="D948" s="4" t="s">
-        <v>1655</v>
-      </c>
-      <c r="E948" s="4" t="s">
-        <v>1652</v>
+      <c r="C948" s="5" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D948" s="5"/>
+      <c r="E948" s="5" t="s">
+        <v>1440</v>
       </c>
       <c r="F948" s="7">
         <v>0</v>
@@ -27607,21 +27615,19 @@
     </row>
     <row r="949" spans="1:7">
       <c r="A949" s="4" t="s">
+        <v>1655</v>
+      </c>
+      <c r="B949" s="5" t="s">
         <v>1656</v>
       </c>
-      <c r="B949" s="5" t="s">
+      <c r="C949" s="4" t="s">
         <v>1657</v>
       </c>
-      <c r="C949" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D949" s="4" t="s">
-        <v>1658</v>
-      </c>
+      <c r="D949" s="5"/>
       <c r="E949" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F949" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F949" s="7">
         <v>0</v>
       </c>
       <c r="G949" s="7">
@@ -27630,21 +27636,21 @@
     </row>
     <row r="950" spans="1:7">
       <c r="A950" s="4" t="s">
+        <v>1658</v>
+      </c>
+      <c r="B950" s="5" t="s">
         <v>1659</v>
       </c>
-      <c r="B950" s="4" t="s">
+      <c r="C950" s="4" t="s">
+        <v>1657</v>
+      </c>
+      <c r="D950" s="4" t="s">
         <v>1660</v>
       </c>
-      <c r="C950" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D950" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="E950" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F950" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F950" s="7">
         <v>0</v>
       </c>
       <c r="G950" s="7">
@@ -27655,15 +27661,17 @@
       <c r="A951" s="4" t="s">
         <v>1661</v>
       </c>
-      <c r="B951" s="4" t="s">
-        <v>1660</v>
+      <c r="B951" s="5" t="s">
+        <v>1662</v>
       </c>
       <c r="C951" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D951" s="5"/>
+        <v>1657</v>
+      </c>
+      <c r="D951" s="4" t="s">
+        <v>1663</v>
+      </c>
       <c r="E951" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F951" s="8">
         <v>0</v>
@@ -27674,19 +27682,21 @@
     </row>
     <row r="952" spans="1:7">
       <c r="A952" s="4" t="s">
-        <v>1662</v>
+        <v>1664</v>
       </c>
       <c r="B952" s="4" t="s">
-        <v>1660</v>
+        <v>1665</v>
       </c>
       <c r="C952" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D952" s="5"/>
+        <v>1657</v>
+      </c>
+      <c r="D952" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E952" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F952" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F952" s="8">
         <v>0</v>
       </c>
       <c r="G952" s="7">
@@ -27695,17 +27705,17 @@
     </row>
     <row r="953" spans="1:7">
       <c r="A953" s="4" t="s">
-        <v>1663</v>
+        <v>1666</v>
       </c>
       <c r="B953" s="4" t="s">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="C953" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D953" s="5"/>
       <c r="E953" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F953" s="8">
         <v>0</v>
@@ -27716,17 +27726,17 @@
     </row>
     <row r="954" spans="1:7">
       <c r="A954" s="4" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B954" s="4" t="s">
         <v>1665</v>
       </c>
-      <c r="B954" s="5" t="s">
-        <v>1666</v>
-      </c>
       <c r="C954" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D954" s="5"/>
       <c r="E954" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F954" s="7">
         <v>0</v>
@@ -27737,17 +27747,17 @@
     </row>
     <row r="955" spans="1:7">
       <c r="A955" s="4" t="s">
-        <v>1667</v>
+        <v>1668</v>
       </c>
       <c r="B955" s="4" t="s">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="C955" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D955" s="5"/>
       <c r="E955" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F955" s="8">
         <v>0</v>
@@ -27758,19 +27768,19 @@
     </row>
     <row r="956" spans="1:7">
       <c r="A956" s="4" t="s">
-        <v>1669</v>
+        <v>1670</v>
       </c>
       <c r="B956" s="5" t="s">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="C956" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D956" s="5"/>
       <c r="E956" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F956" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F956" s="7">
         <v>0</v>
       </c>
       <c r="G956" s="7">
@@ -27779,17 +27789,17 @@
     </row>
     <row r="957" spans="1:7">
       <c r="A957" s="4" t="s">
-        <v>1671</v>
-      </c>
-      <c r="B957" s="5" t="s">
         <v>1672</v>
       </c>
+      <c r="B957" s="4" t="s">
+        <v>1673</v>
+      </c>
       <c r="C957" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D957" s="5"/>
       <c r="E957" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F957" s="8">
         <v>0</v>
@@ -27800,21 +27810,19 @@
     </row>
     <row r="958" spans="1:7">
       <c r="A958" s="4" t="s">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="B958" s="5" t="s">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="C958" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D958" s="4" t="s">
-        <v>1675</v>
-      </c>
+        <v>1657</v>
+      </c>
+      <c r="D958" s="5"/>
       <c r="E958" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F958" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F958" s="8">
         <v>0</v>
       </c>
       <c r="G958" s="7">
@@ -27829,11 +27837,11 @@
         <v>1677</v>
       </c>
       <c r="C959" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D959" s="5"/>
       <c r="E959" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F959" s="8">
         <v>0</v>
@@ -27850,11 +27858,13 @@
         <v>1679</v>
       </c>
       <c r="C960" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D960" s="5"/>
+        <v>1657</v>
+      </c>
+      <c r="D960" s="4" t="s">
+        <v>1680</v>
+      </c>
       <c r="E960" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F960" s="7">
         <v>0</v>
@@ -27865,19 +27875,17 @@
     </row>
     <row r="961" spans="1:7">
       <c r="A961" s="4" t="s">
-        <v>1680</v>
-      </c>
-      <c r="B961" s="4" t="s">
         <v>1681</v>
       </c>
+      <c r="B961" s="5" t="s">
+        <v>1682</v>
+      </c>
       <c r="C961" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D961" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>1657</v>
+      </c>
+      <c r="D961" s="5"/>
       <c r="E961" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F961" s="8">
         <v>0</v>
@@ -27887,18 +27895,18 @@
       </c>
     </row>
     <row r="962" spans="1:7">
-      <c r="A962" s="5" t="s">
-        <v>1682</v>
+      <c r="A962" s="4" t="s">
+        <v>1683</v>
       </c>
       <c r="B962" s="5" t="s">
-        <v>1683</v>
-      </c>
-      <c r="C962" s="5" t="s">
-        <v>1652</v>
+        <v>1684</v>
+      </c>
+      <c r="C962" s="4" t="s">
+        <v>1657</v>
       </c>
       <c r="D962" s="5"/>
-      <c r="E962" s="5" t="s">
-        <v>1652</v>
+      <c r="E962" s="4" t="s">
+        <v>1657</v>
       </c>
       <c r="F962" s="7">
         <v>0</v>
@@ -27909,17 +27917,19 @@
     </row>
     <row r="963" spans="1:7">
       <c r="A963" s="4" t="s">
-        <v>1684</v>
-      </c>
-      <c r="B963" s="5" t="s">
         <v>1685</v>
       </c>
+      <c r="B963" s="4" t="s">
+        <v>1686</v>
+      </c>
       <c r="C963" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D963" s="5"/>
+        <v>1657</v>
+      </c>
+      <c r="D963" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E963" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F963" s="8">
         <v>0</v>
@@ -27929,22 +27939,20 @@
       </c>
     </row>
     <row r="964" spans="1:7">
-      <c r="A964" s="4" t="s">
-        <v>1686</v>
+      <c r="A964" s="5" t="s">
+        <v>1687</v>
       </c>
       <c r="B964" s="5" t="s">
-        <v>1687</v>
-      </c>
-      <c r="C964" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D964" s="5" t="s">
         <v>1688</v>
       </c>
-      <c r="E964" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F964" s="8">
+      <c r="C964" s="5" t="s">
+        <v>1657</v>
+      </c>
+      <c r="D964" s="5"/>
+      <c r="E964" s="5" t="s">
+        <v>1657</v>
+      </c>
+      <c r="F964" s="7">
         <v>0</v>
       </c>
       <c r="G964" s="7">
@@ -27955,15 +27963,15 @@
       <c r="A965" s="4" t="s">
         <v>1689</v>
       </c>
-      <c r="B965" s="4" t="s">
+      <c r="B965" s="5" t="s">
         <v>1690</v>
       </c>
       <c r="C965" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D965" s="5"/>
       <c r="E965" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F965" s="8">
         <v>0</v>
@@ -27976,15 +27984,17 @@
       <c r="A966" s="4" t="s">
         <v>1691</v>
       </c>
-      <c r="B966" s="4" t="s">
+      <c r="B966" s="5" t="s">
         <v>1692</v>
       </c>
       <c r="C966" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D966" s="5"/>
+        <v>1657</v>
+      </c>
+      <c r="D966" s="5" t="s">
+        <v>1693</v>
+      </c>
       <c r="E966" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F966" s="8">
         <v>0</v>
@@ -27995,19 +28005,19 @@
     </row>
     <row r="967" spans="1:7">
       <c r="A967" s="4" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="B967" s="4" t="s">
-        <v>1692</v>
+        <v>1695</v>
       </c>
       <c r="C967" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D967" s="5"/>
       <c r="E967" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F967" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F967" s="8">
         <v>0</v>
       </c>
       <c r="G967" s="7">
@@ -28016,21 +28026,19 @@
     </row>
     <row r="968" spans="1:7">
       <c r="A968" s="4" t="s">
-        <v>1694</v>
-      </c>
-      <c r="B968" s="5" t="s">
-        <v>1695</v>
+        <v>1696</v>
+      </c>
+      <c r="B968" s="4" t="s">
+        <v>1697</v>
       </c>
       <c r="C968" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D968" s="4" t="s">
-        <v>1696</v>
-      </c>
+        <v>1657</v>
+      </c>
+      <c r="D968" s="5"/>
       <c r="E968" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F968" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F968" s="8">
         <v>0</v>
       </c>
       <c r="G968" s="7">
@@ -28039,19 +28047,19 @@
     </row>
     <row r="969" spans="1:7">
       <c r="A969" s="4" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B969" s="4" t="s">
         <v>1697</v>
       </c>
-      <c r="B969" s="5" t="s">
-        <v>1698</v>
-      </c>
       <c r="C969" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D969" s="5"/>
       <c r="E969" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F969" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F969" s="7">
         <v>0</v>
       </c>
       <c r="G969" s="7">
@@ -28066,11 +28074,13 @@
         <v>1700</v>
       </c>
       <c r="C970" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D970" s="5"/>
+        <v>1657</v>
+      </c>
+      <c r="D970" s="4" t="s">
+        <v>1701</v>
+      </c>
       <c r="E970" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F970" s="7">
         <v>0</v>
@@ -28081,17 +28091,17 @@
     </row>
     <row r="971" spans="1:7">
       <c r="A971" s="4" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="B971" s="5" t="s">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="C971" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D971" s="5"/>
       <c r="E971" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F971" s="8">
         <v>0</v>
@@ -28102,21 +28112,19 @@
     </row>
     <row r="972" spans="1:7">
       <c r="A972" s="4" t="s">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="B972" s="5" t="s">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="C972" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D972" s="4" t="s">
-        <v>1705</v>
-      </c>
+        <v>1657</v>
+      </c>
+      <c r="D972" s="5"/>
       <c r="E972" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F972" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F972" s="7">
         <v>0</v>
       </c>
       <c r="G972" s="7">
@@ -28131,11 +28139,11 @@
         <v>1707</v>
       </c>
       <c r="C973" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D973" s="5"/>
       <c r="E973" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F973" s="8">
         <v>0</v>
@@ -28152,15 +28160,15 @@
         <v>1709</v>
       </c>
       <c r="C974" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D974" s="5" t="s">
+        <v>1657</v>
+      </c>
+      <c r="D974" s="4" t="s">
         <v>1710</v>
       </c>
       <c r="E974" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F974" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F974" s="8">
         <v>0</v>
       </c>
       <c r="G974" s="7">
@@ -28175,13 +28183,13 @@
         <v>1712</v>
       </c>
       <c r="C975" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D975" s="5"/>
       <c r="E975" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F975" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F975" s="8">
         <v>0</v>
       </c>
       <c r="G975" s="7">
@@ -28196,13 +28204,15 @@
         <v>1714</v>
       </c>
       <c r="C976" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D976" s="5"/>
+        <v>1657</v>
+      </c>
+      <c r="D976" s="5" t="s">
+        <v>1715</v>
+      </c>
       <c r="E976" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F976" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F976" s="7">
         <v>0</v>
       </c>
       <c r="G976" s="7">
@@ -28211,17 +28221,17 @@
     </row>
     <row r="977" spans="1:7">
       <c r="A977" s="4" t="s">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="B977" s="5" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="C977" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D977" s="5"/>
       <c r="E977" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F977" s="7">
         <v>0</v>
@@ -28232,19 +28242,19 @@
     </row>
     <row r="978" spans="1:7">
       <c r="A978" s="4" t="s">
-        <v>1717</v>
-      </c>
-      <c r="B978" s="4" t="s">
         <v>1718</v>
       </c>
+      <c r="B978" s="5" t="s">
+        <v>1719</v>
+      </c>
       <c r="C978" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D978" s="5"/>
       <c r="E978" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F978" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F978" s="8">
         <v>0</v>
       </c>
       <c r="G978" s="7">
@@ -28253,21 +28263,19 @@
     </row>
     <row r="979" spans="1:7">
       <c r="A979" s="4" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="B979" s="5" t="s">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="C979" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D979" s="4" t="s">
-        <v>1721</v>
-      </c>
+        <v>1657</v>
+      </c>
+      <c r="D979" s="5"/>
       <c r="E979" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F979" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F979" s="7">
         <v>0</v>
       </c>
       <c r="G979" s="7">
@@ -28282,11 +28290,11 @@
         <v>1723</v>
       </c>
       <c r="C980" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D980" s="5"/>
       <c r="E980" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F980" s="7">
         <v>0</v>
@@ -28303,13 +28311,15 @@
         <v>1725</v>
       </c>
       <c r="C981" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D981" s="5"/>
+        <v>1657</v>
+      </c>
+      <c r="D981" s="4" t="s">
+        <v>1726</v>
+      </c>
       <c r="E981" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F981" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F981" s="8">
         <v>0</v>
       </c>
       <c r="G981" s="7">
@@ -28318,19 +28328,19 @@
     </row>
     <row r="982" spans="1:7">
       <c r="A982" s="4" t="s">
-        <v>1726</v>
-      </c>
-      <c r="B982" s="5" t="s">
         <v>1727</v>
       </c>
+      <c r="B982" s="4" t="s">
+        <v>1728</v>
+      </c>
       <c r="C982" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D982" s="5"/>
       <c r="E982" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F982" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F982" s="7">
         <v>0</v>
       </c>
       <c r="G982" s="7">
@@ -28339,17 +28349,17 @@
     </row>
     <row r="983" spans="1:7">
       <c r="A983" s="4" t="s">
-        <v>1728</v>
-      </c>
-      <c r="B983" s="4" t="s">
         <v>1729</v>
       </c>
+      <c r="B983" s="5" t="s">
+        <v>1730</v>
+      </c>
       <c r="C983" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D983" s="5"/>
       <c r="E983" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F983" s="7">
         <v>0</v>
@@ -28360,19 +28370,19 @@
     </row>
     <row r="984" spans="1:7">
       <c r="A984" s="4" t="s">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="B984" s="5" t="s">
-        <v>1731</v>
+        <v>1732</v>
       </c>
       <c r="C984" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D984" s="5"/>
       <c r="E984" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F984" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F984" s="8">
         <v>0</v>
       </c>
       <c r="G984" s="7">
@@ -28381,19 +28391,19 @@
     </row>
     <row r="985" spans="1:7">
       <c r="A985" s="4" t="s">
-        <v>1732</v>
-      </c>
-      <c r="B985" s="5" t="s">
         <v>1733</v>
       </c>
+      <c r="B985" s="4" t="s">
+        <v>1734</v>
+      </c>
       <c r="C985" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D985" s="5"/>
       <c r="E985" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F985" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F985" s="7">
         <v>0</v>
       </c>
       <c r="G985" s="7">
@@ -28402,19 +28412,19 @@
     </row>
     <row r="986" spans="1:7">
       <c r="A986" s="4" t="s">
-        <v>1734</v>
-      </c>
-      <c r="B986" s="4" t="s">
         <v>1735</v>
       </c>
+      <c r="B986" s="5" t="s">
+        <v>1736</v>
+      </c>
       <c r="C986" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D986" s="4"/>
+        <v>1657</v>
+      </c>
+      <c r="D986" s="5"/>
       <c r="E986" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F986" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F986" s="7">
         <v>0</v>
       </c>
       <c r="G986" s="7">
@@ -28423,17 +28433,17 @@
     </row>
     <row r="987" spans="1:7">
       <c r="A987" s="4" t="s">
-        <v>1736</v>
-      </c>
-      <c r="B987" s="4" t="s">
         <v>1737</v>
       </c>
+      <c r="B987" s="5" t="s">
+        <v>1738</v>
+      </c>
       <c r="C987" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D987" s="5"/>
       <c r="E987" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F987" s="8">
         <v>0</v>
@@ -28444,19 +28454,19 @@
     </row>
     <row r="988" spans="1:7">
       <c r="A988" s="4" t="s">
-        <v>1738</v>
+        <v>1739</v>
       </c>
       <c r="B988" s="4" t="s">
-        <v>1739</v>
+        <v>1740</v>
       </c>
       <c r="C988" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D988" s="5"/>
+        <v>1657</v>
+      </c>
+      <c r="D988" s="4"/>
       <c r="E988" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F988" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F988" s="8">
         <v>0</v>
       </c>
       <c r="G988" s="7">
@@ -28465,19 +28475,19 @@
     </row>
     <row r="989" spans="1:7">
       <c r="A989" s="4" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B989" s="5" t="s">
         <v>1741</v>
       </c>
+      <c r="B989" s="4" t="s">
+        <v>1742</v>
+      </c>
       <c r="C989" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D989" s="5"/>
       <c r="E989" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F989" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F989" s="8">
         <v>0</v>
       </c>
       <c r="G989" s="7">
@@ -28485,20 +28495,20 @@
       </c>
     </row>
     <row r="990" spans="1:7">
-      <c r="A990" s="32" t="s">
-        <v>1742</v>
-      </c>
-      <c r="B990" s="33" t="s">
+      <c r="A990" s="4" t="s">
         <v>1743</v>
       </c>
+      <c r="B990" s="4" t="s">
+        <v>1744</v>
+      </c>
       <c r="C990" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D990" s="5"/>
       <c r="E990" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F990" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F990" s="7">
         <v>0</v>
       </c>
       <c r="G990" s="7">
@@ -28506,22 +28516,20 @@
       </c>
     </row>
     <row r="991" spans="1:7">
-      <c r="A991" s="34" t="s">
-        <v>1744</v>
-      </c>
-      <c r="B991" s="4" t="s">
+      <c r="A991" s="4" t="s">
         <v>1745</v>
       </c>
+      <c r="B991" s="5" t="s">
+        <v>1746</v>
+      </c>
       <c r="C991" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D991" s="4" t="s">
-        <v>1746</v>
-      </c>
+        <v>1657</v>
+      </c>
+      <c r="D991" s="5"/>
       <c r="E991" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F991" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F991" s="7">
         <v>0</v>
       </c>
       <c r="G991" s="7">
@@ -28529,20 +28537,20 @@
       </c>
     </row>
     <row r="992" spans="1:7">
-      <c r="A992" s="4" t="s">
+      <c r="A992" s="28" t="s">
         <v>1747</v>
       </c>
-      <c r="B992" s="5" t="s">
+      <c r="B992" s="29" t="s">
         <v>1748</v>
       </c>
       <c r="C992" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D992" s="5"/>
       <c r="E992" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F992" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F992" s="8">
         <v>0</v>
       </c>
       <c r="G992" s="7">
@@ -28550,18 +28558,20 @@
       </c>
     </row>
     <row r="993" spans="1:7">
-      <c r="A993" s="4" t="s">
+      <c r="A993" s="30" t="s">
         <v>1749</v>
       </c>
-      <c r="B993" s="5" t="s">
+      <c r="B993" s="4" t="s">
         <v>1750</v>
       </c>
       <c r="C993" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D993" s="5"/>
+        <v>1657</v>
+      </c>
+      <c r="D993" s="4" t="s">
+        <v>1751</v>
+      </c>
       <c r="E993" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F993" s="8">
         <v>0</v>
@@ -28572,17 +28582,17 @@
     </row>
     <row r="994" spans="1:7">
       <c r="A994" s="4" t="s">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="B994" s="5" t="s">
-        <v>1752</v>
+        <v>1753</v>
       </c>
       <c r="C994" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D994" s="5"/>
       <c r="E994" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F994" s="7">
         <v>0</v>
@@ -28593,17 +28603,17 @@
     </row>
     <row r="995" spans="1:7">
       <c r="A995" s="4" t="s">
-        <v>1753</v>
-      </c>
-      <c r="B995" s="4" t="s">
         <v>1754</v>
       </c>
+      <c r="B995" s="5" t="s">
+        <v>1755</v>
+      </c>
       <c r="C995" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D995" s="5"/>
       <c r="E995" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F995" s="8">
         <v>0</v>
@@ -28614,19 +28624,19 @@
     </row>
     <row r="996" spans="1:7">
       <c r="A996" s="4" t="s">
-        <v>1755</v>
+        <v>1756</v>
       </c>
       <c r="B996" s="5" t="s">
-        <v>1756</v>
+        <v>1757</v>
       </c>
       <c r="C996" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D996" s="5"/>
       <c r="E996" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F996" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F996" s="7">
         <v>0</v>
       </c>
       <c r="G996" s="7">
@@ -28635,21 +28645,19 @@
     </row>
     <row r="997" spans="1:7">
       <c r="A997" s="4" t="s">
-        <v>1757</v>
+        <v>1758</v>
       </c>
       <c r="B997" s="4" t="s">
-        <v>1756</v>
+        <v>1759</v>
       </c>
       <c r="C997" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D997" s="4" t="s">
-        <v>1758</v>
-      </c>
+        <v>1657</v>
+      </c>
+      <c r="D997" s="5"/>
       <c r="E997" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F997" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F997" s="8">
         <v>0</v>
       </c>
       <c r="G997" s="7">
@@ -28658,19 +28666,19 @@
     </row>
     <row r="998" spans="1:7">
       <c r="A998" s="4" t="s">
-        <v>1759</v>
+        <v>1760</v>
       </c>
       <c r="B998" s="5" t="s">
-        <v>1760</v>
+        <v>1761</v>
       </c>
       <c r="C998" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D998" s="5"/>
       <c r="E998" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F998" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F998" s="8">
         <v>0</v>
       </c>
       <c r="G998" s="7">
@@ -28679,17 +28687,19 @@
     </row>
     <row r="999" spans="1:7">
       <c r="A999" s="4" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B999" s="4" t="s">
         <v>1761</v>
       </c>
-      <c r="B999" s="4" t="s">
-        <v>1762</v>
-      </c>
       <c r="C999" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D999" s="5"/>
+        <v>1657</v>
+      </c>
+      <c r="D999" s="4" t="s">
+        <v>1763</v>
+      </c>
       <c r="E999" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F999" s="7">
         <v>0</v>
@@ -28700,19 +28710,17 @@
     </row>
     <row r="1000" spans="1:7">
       <c r="A1000" s="4" t="s">
-        <v>1763</v>
-      </c>
-      <c r="B1000" s="4" t="s">
-        <v>1762</v>
+        <v>1764</v>
+      </c>
+      <c r="B1000" s="5" t="s">
+        <v>1765</v>
       </c>
       <c r="C1000" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D1000" s="4" t="s">
-        <v>1764</v>
-      </c>
+        <v>1657</v>
+      </c>
+      <c r="D1000" s="5"/>
       <c r="E1000" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F1000" s="7">
         <v>0</v>
@@ -28723,21 +28731,19 @@
     </row>
     <row r="1001" spans="1:7">
       <c r="A1001" s="4" t="s">
-        <v>1765</v>
+        <v>1766</v>
       </c>
       <c r="B1001" s="4" t="s">
-        <v>1762</v>
+        <v>1767</v>
       </c>
       <c r="C1001" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D1001" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>1657</v>
+      </c>
+      <c r="D1001" s="5"/>
       <c r="E1001" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F1001" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F1001" s="7">
         <v>0</v>
       </c>
       <c r="G1001" s="7">
@@ -28746,21 +28752,21 @@
     </row>
     <row r="1002" spans="1:7">
       <c r="A1002" s="4" t="s">
-        <v>1766</v>
+        <v>1768</v>
       </c>
       <c r="B1002" s="4" t="s">
-        <v>1762</v>
+        <v>1767</v>
       </c>
       <c r="C1002" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D1002" s="4" t="s">
-        <v>1767</v>
+        <v>1769</v>
       </c>
       <c r="E1002" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F1002" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F1002" s="7">
         <v>0</v>
       </c>
       <c r="G1002" s="7">
@@ -28769,21 +28775,21 @@
     </row>
     <row r="1003" spans="1:7">
       <c r="A1003" s="4" t="s">
-        <v>1768</v>
+        <v>1770</v>
       </c>
       <c r="B1003" s="4" t="s">
-        <v>1762</v>
+        <v>1767</v>
       </c>
       <c r="C1003" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="D1003" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E1003" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="F1003" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F1003" s="8">
         <v>0</v>
       </c>
       <c r="G1003" s="7">
@@ -28791,18 +28797,20 @@
       </c>
     </row>
     <row r="1004" spans="1:7">
-      <c r="A1004" s="5" t="s">
-        <v>1769</v>
+      <c r="A1004" s="4" t="s">
+        <v>1771</v>
       </c>
       <c r="B1004" s="4" t="s">
-        <v>1770</v>
+        <v>1767</v>
       </c>
       <c r="C1004" s="4" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D1004" s="5"/>
+        <v>1657</v>
+      </c>
+      <c r="D1004" s="4" t="s">
+        <v>1772</v>
+      </c>
       <c r="E1004" s="4" t="s">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="F1004" s="8">
         <v>0</v>
@@ -28813,19 +28821,21 @@
     </row>
     <row r="1005" spans="1:7">
       <c r="A1005" s="4" t="s">
-        <v>426</v>
+        <v>1773</v>
       </c>
       <c r="B1005" s="4" t="s">
-        <v>427</v>
+        <v>1767</v>
       </c>
       <c r="C1005" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="D1005" s="5"/>
+        <v>1657</v>
+      </c>
+      <c r="D1005" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E1005" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="F1005" s="8">
+        <v>1657</v>
+      </c>
+      <c r="F1005" s="7">
         <v>0</v>
       </c>
       <c r="G1005" s="7">
@@ -28833,20 +28843,20 @@
       </c>
     </row>
     <row r="1006" spans="1:7">
-      <c r="A1006" s="4" t="s">
-        <v>1772</v>
+      <c r="A1006" s="5" t="s">
+        <v>1774</v>
       </c>
       <c r="B1006" s="4" t="s">
-        <v>1773</v>
+        <v>1775</v>
       </c>
       <c r="C1006" s="4" t="s">
-        <v>1771</v>
+        <v>1657</v>
       </c>
       <c r="D1006" s="5"/>
       <c r="E1006" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="F1006" s="7">
+        <v>1657</v>
+      </c>
+      <c r="F1006" s="8">
         <v>0</v>
       </c>
       <c r="G1006" s="7">
@@ -28855,20 +28865,20 @@
     </row>
     <row r="1007" spans="1:7">
       <c r="A1007" s="4" t="s">
-        <v>1774</v>
+        <v>1776</v>
       </c>
       <c r="B1007" s="4" t="s">
-        <v>1775</v>
+        <v>309</v>
       </c>
       <c r="C1007" s="4" t="s">
-        <v>1771</v>
+        <v>1657</v>
       </c>
       <c r="D1007" s="5"/>
       <c r="E1007" s="4" t="s">
-        <v>1771</v>
+        <v>1657</v>
       </c>
       <c r="F1007" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1007" s="7">
         <v>0</v>
@@ -28876,19 +28886,19 @@
     </row>
     <row r="1008" spans="1:7">
       <c r="A1008" s="4" t="s">
-        <v>1776</v>
+        <v>426</v>
       </c>
       <c r="B1008" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="C1008" s="4" t="s">
         <v>1777</v>
-      </c>
-      <c r="C1008" s="4" t="s">
-        <v>1771</v>
       </c>
       <c r="D1008" s="5"/>
       <c r="E1008" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="F1008" s="7">
+        <v>1777</v>
+      </c>
+      <c r="F1008" s="8">
         <v>0</v>
       </c>
       <c r="G1008" s="7">
@@ -28903,15 +28913,13 @@
         <v>1779</v>
       </c>
       <c r="C1009" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="D1009" s="4" t="s">
-        <v>14</v>
-      </c>
+        <v>1777</v>
+      </c>
+      <c r="D1009" s="5"/>
       <c r="E1009" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="F1009" s="8">
+        <v>1777</v>
+      </c>
+      <c r="F1009" s="7">
         <v>0</v>
       </c>
       <c r="G1009" s="7">
@@ -28923,18 +28931,16 @@
         <v>1780</v>
       </c>
       <c r="B1010" s="4" t="s">
-        <v>381</v>
+        <v>1781</v>
       </c>
       <c r="C1010" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="D1010" s="4" t="s">
-        <v>14</v>
-      </c>
+        <v>1777</v>
+      </c>
+      <c r="D1010" s="5"/>
       <c r="E1010" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="F1010" s="8">
+        <v>1777</v>
+      </c>
+      <c r="F1010" s="7">
         <v>0</v>
       </c>
       <c r="G1010" s="7">
@@ -28943,17 +28949,17 @@
     </row>
     <row r="1011" spans="1:7">
       <c r="A1011" s="4" t="s">
-        <v>1781</v>
+        <v>1782</v>
       </c>
       <c r="B1011" s="4" t="s">
-        <v>381</v>
+        <v>1783</v>
       </c>
       <c r="C1011" s="4" t="s">
-        <v>1771</v>
+        <v>1777</v>
       </c>
       <c r="D1011" s="5"/>
       <c r="E1011" s="4" t="s">
-        <v>1771</v>
+        <v>1777</v>
       </c>
       <c r="F1011" s="7">
         <v>0</v>
@@ -28964,21 +28970,21 @@
     </row>
     <row r="1012" spans="1:7">
       <c r="A1012" s="4" t="s">
-        <v>1782</v>
+        <v>1784</v>
       </c>
       <c r="B1012" s="4" t="s">
-        <v>20</v>
+        <v>1785</v>
       </c>
       <c r="C1012" s="4" t="s">
-        <v>1771</v>
+        <v>1777</v>
       </c>
       <c r="D1012" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E1012" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="F1012" s="7">
+        <v>1777</v>
+      </c>
+      <c r="F1012" s="8">
         <v>0</v>
       </c>
       <c r="G1012" s="7">
@@ -28987,19 +28993,19 @@
     </row>
     <row r="1013" spans="1:7">
       <c r="A1013" s="4" t="s">
-        <v>1783</v>
+        <v>1786</v>
       </c>
       <c r="B1013" s="4" t="s">
-        <v>1784</v>
+        <v>381</v>
       </c>
       <c r="C1013" s="4" t="s">
-        <v>1771</v>
+        <v>1777</v>
       </c>
       <c r="D1013" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E1013" s="4" t="s">
-        <v>1771</v>
+        <v>1777</v>
       </c>
       <c r="F1013" s="8">
         <v>0</v>
@@ -29010,21 +29016,19 @@
     </row>
     <row r="1014" spans="1:7">
       <c r="A1014" s="4" t="s">
-        <v>1785</v>
+        <v>1787</v>
       </c>
       <c r="B1014" s="4" t="s">
-        <v>1786</v>
+        <v>381</v>
       </c>
       <c r="C1014" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="D1014" s="4" t="s">
-        <v>14</v>
-      </c>
+        <v>1777</v>
+      </c>
+      <c r="D1014" s="5"/>
       <c r="E1014" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="F1014" s="8">
+        <v>1777</v>
+      </c>
+      <c r="F1014" s="7">
         <v>0</v>
       </c>
       <c r="G1014" s="7">
@@ -29033,17 +29037,19 @@
     </row>
     <row r="1015" spans="1:7">
       <c r="A1015" s="4" t="s">
-        <v>1787</v>
+        <v>1788</v>
       </c>
       <c r="B1015" s="4" t="s">
-        <v>1788</v>
+        <v>20</v>
       </c>
       <c r="C1015" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="D1015" s="5"/>
+        <v>1777</v>
+      </c>
+      <c r="D1015" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="E1015" s="4" t="s">
-        <v>1771</v>
+        <v>1777</v>
       </c>
       <c r="F1015" s="7">
         <v>0</v>
@@ -29056,15 +29062,17 @@
       <c r="A1016" s="4" t="s">
         <v>1789</v>
       </c>
-      <c r="B1016" s="5" t="s">
+      <c r="B1016" s="4" t="s">
         <v>1790</v>
       </c>
       <c r="C1016" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="D1016" s="4"/>
+        <v>1777</v>
+      </c>
+      <c r="D1016" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="E1016" s="4" t="s">
-        <v>1771</v>
+        <v>1777</v>
       </c>
       <c r="F1016" s="8">
         <v>0</v>
@@ -29081,13 +29089,15 @@
         <v>1792</v>
       </c>
       <c r="C1017" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="D1017" s="5"/>
+        <v>1777</v>
+      </c>
+      <c r="D1017" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="E1017" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="F1017" s="7">
+        <v>1777</v>
+      </c>
+      <c r="F1017" s="8">
         <v>0</v>
       </c>
       <c r="G1017" s="7">
@@ -29102,11 +29112,11 @@
         <v>1794</v>
       </c>
       <c r="C1018" s="4" t="s">
-        <v>1771</v>
+        <v>1777</v>
       </c>
       <c r="D1018" s="5"/>
       <c r="E1018" s="4" t="s">
-        <v>1771</v>
+        <v>1777</v>
       </c>
       <c r="F1018" s="7">
         <v>0</v>
@@ -29119,15 +29129,15 @@
       <c r="A1019" s="4" t="s">
         <v>1795</v>
       </c>
-      <c r="B1019" s="4" t="s">
+      <c r="B1019" s="5" t="s">
         <v>1796</v>
       </c>
       <c r="C1019" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="D1019" s="5"/>
+        <v>1777</v>
+      </c>
+      <c r="D1019" s="4"/>
       <c r="E1019" s="4" t="s">
-        <v>1771</v>
+        <v>1777</v>
       </c>
       <c r="F1019" s="8">
         <v>0</v>
@@ -29141,25 +29151,89 @@
         <v>1797</v>
       </c>
       <c r="B1020" s="4" t="s">
-        <v>1796</v>
+        <v>1798</v>
       </c>
       <c r="C1020" s="4" t="s">
-        <v>1771</v>
+        <v>1777</v>
       </c>
       <c r="D1020" s="5"/>
       <c r="E1020" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="F1020" s="8">
+        <v>1777</v>
+      </c>
+      <c r="F1020" s="7">
         <v>0</v>
       </c>
       <c r="G1020" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:7">
+      <c r="A1021" s="4" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B1021" s="4" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C1021" s="4" t="s">
+        <v>1777</v>
+      </c>
+      <c r="D1021" s="5"/>
+      <c r="E1021" s="4" t="s">
+        <v>1777</v>
+      </c>
+      <c r="F1021" s="7">
+        <v>0</v>
+      </c>
+      <c r="G1021" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:7">
+      <c r="A1022" s="4" t="s">
+        <v>1801</v>
+      </c>
+      <c r="B1022" s="4" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C1022" s="4" t="s">
+        <v>1777</v>
+      </c>
+      <c r="D1022" s="5"/>
+      <c r="E1022" s="4" t="s">
+        <v>1777</v>
+      </c>
+      <c r="F1022" s="8">
+        <v>0</v>
+      </c>
+      <c r="G1022" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:7">
+      <c r="A1023" s="4" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B1023" s="4" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C1023" s="4" t="s">
+        <v>1777</v>
+      </c>
+      <c r="D1023" s="5"/>
+      <c r="E1023" s="4" t="s">
+        <v>1777</v>
+      </c>
+      <c r="F1023" s="8">
+        <v>0</v>
+      </c>
+      <c r="G1023" s="7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" insertHyperlinks="0" autoFilter="0"/>
-  <sortState ref="A2:G1020">
+  <autoFilter ref="A1:G1023"/>
+  <sortState ref="A2:G1023">
     <sortCondition ref="E1"/>
   </sortState>
   <dataValidations count="1">
@@ -29171,7 +29245,7 @@
     <hyperlink ref="D889" r:id="rId1" display="《国王排名》ED" tooltip="https://baike.baidu.com/item/%E5%9B%BD%E7%8E%8B%E6%8E%92%E5%90%8D/24190907"/>
     <hyperlink ref="D201" r:id="rId2" display="《英雄联盟：双城之战》的中文主题曲" tooltip="https://baike.baidu.com/item/%E8%8B%B1%E9%9B%84%E8%81%94%E7%9B%9F%EF%BC%9A%E5%8F%8C%E5%9F%8E%E4%B9%8B%E6%88%98/58613563"/>
     <hyperlink ref="D866" r:id="rId3" display="我的世界已坠入爱河《闪烁的青春》OP主题曲" tooltip="https://baike.baidu.com/item/%E9%97%AA%E7%83%81%E7%9A%84%E9%9D%92%E6%98%A5/13320086"/>
-    <hyperlink ref="D937" r:id="rId4" display="《明日方舟》EP" tooltip="https://baike.baidu.com/item/%E9%AC%BC%E7%81%AD%E4%B9%8B%E5%88%83%EF%BC%9A%E6%97%A0%E9%99%90%E5%88%97%E8%BD%A6%E7%AF%87/23783245"/>
+    <hyperlink ref="D939" r:id="rId4" display="《明日方舟》EP" tooltip="https://baike.baidu.com/item/%E9%AC%BC%E7%81%AD%E4%B9%8B%E5%88%83%EF%BC%9A%E6%97%A0%E9%99%90%E5%88%97%E8%BD%A6%E7%AF%87/23783245"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -29185,8 +29259,20 @@
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <autofilters xmlns="https://web.wps.cn/et/2018/main">
   <sheetItem sheetStid="1">
-    <filterData filterID="1331220589"/>
+    <filterData filterID="1331220589">
+      <hiddenRange rowFrom="1" rowTo="38"/>
+      <hiddenRange rowFrom="40" rowTo="1022"/>
+    </filterData>
     <filterData filterID="1331040869"/>
+    <autofilterInfo filterID="1331220589">
+      <autoFilter xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G1023">
+        <filterColumn colId="0">
+          <customFilters>
+            <customFilter operator="equal" val="百变奶精"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
+    </autofilterInfo>
   </sheetItem>
 </autofilters>
 </file>
@@ -29194,7 +29280,9 @@
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <woProps xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <woSheetsProps>
-    <woSheetProps sheetStid="1" interlineOnOff="0" interlineColor="0" isDbSheet="0" isDashBoardSheet="0"/>
+    <woSheetProps sheetStid="1" interlineOnOff="0" interlineColor="0" isDbSheet="0" isDashBoardSheet="0">
+      <cellprotection/>
+    </woSheetProps>
   </woSheetsProps>
   <woBookProps>
     <bookSettings isFilterShared="0" coreConquerUserId="" isAutoUpdatePaused="0" filterType="user" isMergeTasksAutoUpdate="0" isInserPicAsAttachment="0"/>

</xml_diff>

<commit_message>
updated song list 2022/6/9 2
</commit_message>
<xml_diff>
--- a/music_list_7.xlsx
+++ b/music_list_7.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4920" uniqueCount="1987">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4925" uniqueCount="1989">
   <si>
     <t>歌名</t>
   </si>
@@ -5440,6 +5440,12 @@
     <t>《白色相簿2》OP</t>
   </si>
   <si>
+    <t>さよならのこと</t>
+  </si>
+  <si>
+    <t>《WHITE Album》</t>
+  </si>
+  <si>
     <t>扉を開けて/敞开心扉</t>
   </si>
   <si>
@@ -6042,45 +6048,45 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="39">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
-    <numFmt numFmtId="177" formatCode="#\ ??/??"/>
-    <numFmt numFmtId="178" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
+    <numFmt numFmtId="177" formatCode="mmmm\-yy"/>
     <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
     <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="178" formatCode="\¥#,##0;\¥\-#,##0"/>
+    <numFmt numFmtId="179" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="180" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="181" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="182" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="183" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
+    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="184" formatCode="dd\-mmm\-yy"/>
     <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
+    <numFmt numFmtId="185" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="186" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="187" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
+    <numFmt numFmtId="188" formatCode="yy/m/d"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="189" formatCode="m/d"/>
+    <numFmt numFmtId="190" formatCode="#\ ??"/>
+    <numFmt numFmtId="191" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="192" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="193" formatCode="#\ ??/??"/>
+    <numFmt numFmtId="194" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="195" formatCode="mmmmm"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="196" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+    <numFmt numFmtId="197" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="198" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
+    <numFmt numFmtId="199" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="200" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="201" formatCode="mmmmm\-yy"/>
     <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="179" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="180" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="181" formatCode="h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="182" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="183" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="184" formatCode="#\ ??"/>
-    <numFmt numFmtId="185" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="186" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="187" formatCode="m/d"/>
-    <numFmt numFmtId="188" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="189" formatCode="yy/m/d"/>
-    <numFmt numFmtId="190" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="191" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="192" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="193" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="194" formatCode="mmmmm"/>
-    <numFmt numFmtId="195" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="196" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="197" formatCode="#\ ?/?"/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="198" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="199" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
-    <numFmt numFmtId="200" formatCode="[$-804]aaa"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="201" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="202" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
+    <numFmt numFmtId="202" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="47">
     <font>
@@ -6255,8 +6261,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6269,24 +6298,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6301,7 +6330,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -6310,20 +6339,36 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -6339,24 +6384,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6370,30 +6399,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6427,7 +6433,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6439,31 +6541,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6475,19 +6559,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6499,43 +6571,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6547,13 +6583,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6565,49 +6607,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6618,30 +6624,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -6663,17 +6645,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6693,6 +6669,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -6708,13 +6695,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6723,148 +6729,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="200" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="192" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -6875,7 +6881,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="198" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -6893,10 +6899,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="198" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="191" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="198" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
@@ -7305,9 +7311,9 @@
   <dimension ref="A1:H1079"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1062" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1064" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B1074" sqref="B1074"/>
+      <selection pane="bottomLeft" activeCell="B1079" sqref="B1079"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -30111,30 +30117,31 @@
       </c>
       <c r="H986" s="6"/>
     </row>
-    <row r="987" spans="1:8">
-      <c r="A987" s="5" t="s">
+    <row r="987" spans="1:7">
+      <c r="A987" s="11" t="s">
         <v>1788</v>
       </c>
-      <c r="B987" s="6" t="s">
+      <c r="B987" s="5" t="s">
+        <v>1786</v>
+      </c>
+      <c r="C987" s="11" t="s">
+        <v>1541</v>
+      </c>
+      <c r="D987" s="11" t="s">
         <v>1789</v>
       </c>
-      <c r="C987" s="5" t="s">
+      <c r="E987" s="11" t="s">
         <v>1541</v>
       </c>
-      <c r="D987" s="6"/>
-      <c r="E987" s="5" t="s">
-        <v>1541</v>
-      </c>
-      <c r="F987" s="8">
-        <v>0</v>
-      </c>
-      <c r="G987" s="8">
-        <v>0</v>
-      </c>
-      <c r="H987" s="6"/>
-    </row>
-    <row r="988" spans="1:7">
-      <c r="A988" s="6" t="s">
+      <c r="F987" s="2">
+        <v>1</v>
+      </c>
+      <c r="G987" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="988" spans="1:8">
+      <c r="A988" s="5" t="s">
         <v>1790</v>
       </c>
       <c r="B988" s="6" t="s">
@@ -30143,9 +30150,7 @@
       <c r="C988" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="D988" s="6" t="s">
-        <v>1792</v>
-      </c>
+      <c r="D988" s="6"/>
       <c r="E988" s="5" t="s">
         <v>1541</v>
       </c>
@@ -30155,48 +30160,48 @@
       <c r="G988" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="989" spans="1:8">
-      <c r="A989" s="5" t="s">
+      <c r="H988" s="6"/>
+    </row>
+    <row r="989" spans="1:7">
+      <c r="A989" s="6" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B989" s="6" t="s">
         <v>1793</v>
-      </c>
-      <c r="B989" s="5" t="s">
-        <v>1794</v>
       </c>
       <c r="C989" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="D989" s="5" t="s">
-        <v>1795</v>
+      <c r="D989" s="6" t="s">
+        <v>1794</v>
       </c>
       <c r="E989" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="F989" s="9">
+      <c r="F989" s="8">
         <v>0</v>
       </c>
       <c r="G989" s="8">
         <v>0</v>
       </c>
-      <c r="H989" s="6"/>
     </row>
     <row r="990" spans="1:8">
-      <c r="A990" s="6" t="s">
+      <c r="A990" s="5" t="s">
+        <v>1795</v>
+      </c>
+      <c r="B990" s="5" t="s">
         <v>1796</v>
-      </c>
-      <c r="B990" s="27" t="s">
-        <v>1797</v>
       </c>
       <c r="C990" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="D990" s="30" t="s">
-        <v>1798</v>
+      <c r="D990" s="5" t="s">
+        <v>1797</v>
       </c>
       <c r="E990" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="F990" s="8">
+      <c r="F990" s="9">
         <v>0</v>
       </c>
       <c r="G990" s="8">
@@ -30205,20 +30210,22 @@
       <c r="H990" s="6"/>
     </row>
     <row r="991" spans="1:8">
-      <c r="A991" s="5" t="s">
+      <c r="A991" s="6" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B991" s="27" t="s">
         <v>1799</v>
-      </c>
-      <c r="B991" s="5" t="s">
-        <v>1800</v>
       </c>
       <c r="C991" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="D991" s="6"/>
+      <c r="D991" s="30" t="s">
+        <v>1800</v>
+      </c>
       <c r="E991" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="F991" s="9">
+      <c r="F991" s="8">
         <v>0</v>
       </c>
       <c r="G991" s="8">
@@ -30231,14 +30238,12 @@
         <v>1801</v>
       </c>
       <c r="B992" s="5" t="s">
-        <v>1800</v>
+        <v>1802</v>
       </c>
       <c r="C992" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="D992" s="5" t="s">
-        <v>1802</v>
-      </c>
+      <c r="D992" s="6"/>
       <c r="E992" s="5" t="s">
         <v>1541</v>
       </c>
@@ -30255,18 +30260,18 @@
         <v>1803</v>
       </c>
       <c r="B993" s="5" t="s">
-        <v>1804</v>
+        <v>1802</v>
       </c>
       <c r="C993" s="5" t="s">
         <v>1541</v>
       </c>
       <c r="D993" s="5" t="s">
-        <v>1774</v>
+        <v>1804</v>
       </c>
       <c r="E993" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="F993" s="8">
+      <c r="F993" s="9">
         <v>0</v>
       </c>
       <c r="G993" s="8">
@@ -30285,7 +30290,7 @@
         <v>1541</v>
       </c>
       <c r="D994" s="5" t="s">
-        <v>1807</v>
+        <v>1774</v>
       </c>
       <c r="E994" s="5" t="s">
         <v>1541</v>
@@ -30300,15 +30305,17 @@
     </row>
     <row r="995" spans="1:8">
       <c r="A995" s="5" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B995" s="5" t="s">
         <v>1808</v>
-      </c>
-      <c r="B995" s="6" t="s">
-        <v>1809</v>
       </c>
       <c r="C995" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="D995" s="6"/>
+      <c r="D995" s="5" t="s">
+        <v>1809</v>
+      </c>
       <c r="E995" s="5" t="s">
         <v>1541</v>
       </c>
@@ -30324,15 +30331,13 @@
       <c r="A996" s="5" t="s">
         <v>1810</v>
       </c>
-      <c r="B996" s="5" t="s">
+      <c r="B996" s="6" t="s">
         <v>1811</v>
       </c>
       <c r="C996" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="D996" s="5" t="s">
-        <v>1812</v>
-      </c>
+      <c r="D996" s="6"/>
       <c r="E996" s="5" t="s">
         <v>1541</v>
       </c>
@@ -30345,17 +30350,19 @@
       <c r="H996" s="6"/>
     </row>
     <row r="997" spans="1:8">
-      <c r="A997" s="6" t="s">
+      <c r="A997" s="5" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B997" s="5" t="s">
         <v>1813</v>
       </c>
-      <c r="B997" s="6" t="s">
-        <v>1811</v>
-      </c>
-      <c r="C997" s="6" t="s">
+      <c r="C997" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="D997" s="6"/>
-      <c r="E997" s="6" t="s">
+      <c r="D997" s="5" t="s">
+        <v>1814</v>
+      </c>
+      <c r="E997" s="5" t="s">
         <v>1541</v>
       </c>
       <c r="F997" s="8">
@@ -30368,18 +30375,16 @@
     </row>
     <row r="998" spans="1:8">
       <c r="A998" s="6" t="s">
-        <v>1814</v>
-      </c>
-      <c r="B998" s="5" t="s">
-        <v>1811</v>
-      </c>
-      <c r="C998" s="5" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B998" s="6" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C998" s="6" t="s">
         <v>1541</v>
       </c>
-      <c r="D998" s="6" t="s">
-        <v>1815</v>
-      </c>
-      <c r="E998" s="5" t="s">
+      <c r="D998" s="6"/>
+      <c r="E998" s="6" t="s">
         <v>1541</v>
       </c>
       <c r="F998" s="8">
@@ -30391,17 +30396,17 @@
       <c r="H998" s="6"/>
     </row>
     <row r="999" spans="1:8">
-      <c r="A999" s="5" t="s">
+      <c r="A999" s="6" t="s">
         <v>1816</v>
       </c>
       <c r="B999" s="5" t="s">
-        <v>1817</v>
+        <v>1813</v>
       </c>
       <c r="C999" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="D999" s="5" t="s">
-        <v>1818</v>
+      <c r="D999" s="6" t="s">
+        <v>1817</v>
       </c>
       <c r="E999" s="5" t="s">
         <v>1541</v>
@@ -30416,16 +30421,16 @@
     </row>
     <row r="1000" spans="1:8">
       <c r="A1000" s="5" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B1000" s="5" t="s">
         <v>1819</v>
-      </c>
-      <c r="B1000" s="5" t="s">
-        <v>1820</v>
       </c>
       <c r="C1000" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="D1000" s="30" t="s">
-        <v>1821</v>
+      <c r="D1000" s="5" t="s">
+        <v>1820</v>
       </c>
       <c r="E1000" s="5" t="s">
         <v>1541</v>
@@ -30440,16 +30445,18 @@
     </row>
     <row r="1001" spans="1:8">
       <c r="A1001" s="5" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B1001" s="5" t="s">
         <v>1822</v>
       </c>
-      <c r="B1001" s="6" t="s">
-        <v>1820</v>
-      </c>
-      <c r="C1001" s="6" t="s">
+      <c r="C1001" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="D1001" s="6"/>
-      <c r="E1001" s="6" t="s">
+      <c r="D1001" s="30" t="s">
+        <v>1823</v>
+      </c>
+      <c r="E1001" s="5" t="s">
         <v>1541</v>
       </c>
       <c r="F1001" s="8">
@@ -30458,47 +30465,45 @@
       <c r="G1001" s="8">
         <v>0</v>
       </c>
-      <c r="H1001" s="6" t="s">
-        <v>1823</v>
-      </c>
+      <c r="H1001" s="6"/>
     </row>
     <row r="1002" spans="1:8">
       <c r="A1002" s="5" t="s">
         <v>1824</v>
       </c>
       <c r="B1002" s="6" t="s">
+        <v>1822</v>
+      </c>
+      <c r="C1002" s="6" t="s">
+        <v>1541</v>
+      </c>
+      <c r="D1002" s="6"/>
+      <c r="E1002" s="6" t="s">
+        <v>1541</v>
+      </c>
+      <c r="F1002" s="8">
+        <v>0</v>
+      </c>
+      <c r="G1002" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1002" s="6" t="s">
         <v>1825</v>
       </c>
-      <c r="C1002" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1002" s="6"/>
-      <c r="E1002" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1002" s="8">
-        <v>0</v>
-      </c>
-      <c r="G1002" s="8">
-        <v>0</v>
-      </c>
-      <c r="H1002" s="6"/>
     </row>
     <row r="1003" spans="1:8">
       <c r="A1003" s="5" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B1003" s="6" t="s">
         <v>1827</v>
       </c>
-      <c r="B1003" s="6" t="s">
+      <c r="C1003" s="5" t="s">
         <v>1828</v>
       </c>
-      <c r="C1003" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1003" s="5" t="s">
-        <v>1829</v>
-      </c>
+      <c r="D1003" s="6"/>
       <c r="E1003" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1003" s="8">
         <v>0</v>
@@ -30510,21 +30515,21 @@
     </row>
     <row r="1004" spans="1:8">
       <c r="A1004" s="5" t="s">
+        <v>1829</v>
+      </c>
+      <c r="B1004" s="6" t="s">
         <v>1830</v>
       </c>
-      <c r="B1004" s="6" t="s">
+      <c r="C1004" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1004" s="5" t="s">
         <v>1831</v>
       </c>
-      <c r="C1004" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1004" s="5" t="s">
-        <v>1832</v>
-      </c>
       <c r="E1004" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1004" s="9">
+        <v>1828</v>
+      </c>
+      <c r="F1004" s="8">
         <v>0</v>
       </c>
       <c r="G1004" s="8">
@@ -30534,19 +30539,19 @@
     </row>
     <row r="1005" spans="1:8">
       <c r="A1005" s="5" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B1005" s="6" t="s">
         <v>1833</v>
       </c>
-      <c r="B1005" s="5" t="s">
+      <c r="C1005" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1005" s="5" t="s">
         <v>1834</v>
       </c>
-      <c r="C1005" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1005" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="E1005" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1005" s="9">
         <v>0</v>
@@ -30561,14 +30566,16 @@
         <v>1835</v>
       </c>
       <c r="B1006" s="5" t="s">
-        <v>1834</v>
+        <v>1836</v>
       </c>
       <c r="C1006" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1006" s="6"/>
+        <v>1828</v>
+      </c>
+      <c r="D1006" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E1006" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1006" s="9">
         <v>0</v>
@@ -30580,65 +30587,65 @@
     </row>
     <row r="1007" spans="1:8">
       <c r="A1007" s="5" t="s">
+        <v>1837</v>
+      </c>
+      <c r="B1007" s="5" t="s">
         <v>1836</v>
       </c>
-      <c r="B1007" s="5" t="s">
-        <v>1834</v>
-      </c>
       <c r="C1007" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1007" s="6"/>
       <c r="E1007" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1007" s="8">
+        <v>1828</v>
+      </c>
+      <c r="F1007" s="9">
         <v>0</v>
       </c>
       <c r="G1007" s="8">
         <v>0</v>
       </c>
-      <c r="H1007" s="6" t="s">
-        <v>1837</v>
-      </c>
+      <c r="H1007" s="6"/>
     </row>
     <row r="1008" spans="1:8">
       <c r="A1008" s="5" t="s">
         <v>1838</v>
       </c>
       <c r="B1008" s="5" t="s">
-        <v>1839</v>
+        <v>1836</v>
       </c>
       <c r="C1008" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1008" s="6"/>
       <c r="E1008" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1008" s="9">
+        <v>1828</v>
+      </c>
+      <c r="F1008" s="8">
         <v>0</v>
       </c>
       <c r="G1008" s="8">
         <v>0</v>
       </c>
-      <c r="H1008" s="6"/>
+      <c r="H1008" s="6" t="s">
+        <v>1839</v>
+      </c>
     </row>
     <row r="1009" spans="1:8">
       <c r="A1009" s="5" t="s">
         <v>1840</v>
       </c>
-      <c r="B1009" s="6" t="s">
+      <c r="B1009" s="5" t="s">
         <v>1841</v>
       </c>
       <c r="C1009" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1009" s="6"/>
       <c r="E1009" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1009" s="8">
+        <v>1828</v>
+      </c>
+      <c r="F1009" s="9">
         <v>0</v>
       </c>
       <c r="G1009" s="8">
@@ -30650,17 +30657,17 @@
       <c r="A1010" s="5" t="s">
         <v>1842</v>
       </c>
-      <c r="B1010" s="5" t="s">
+      <c r="B1010" s="6" t="s">
         <v>1843</v>
       </c>
       <c r="C1010" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1010" s="6"/>
       <c r="E1010" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1010" s="9">
+        <v>1828</v>
+      </c>
+      <c r="F1010" s="8">
         <v>0</v>
       </c>
       <c r="G1010" s="8">
@@ -30672,15 +30679,15 @@
       <c r="A1011" s="5" t="s">
         <v>1844</v>
       </c>
-      <c r="B1011" s="6" t="s">
+      <c r="B1011" s="5" t="s">
         <v>1845</v>
       </c>
       <c r="C1011" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1011" s="6"/>
       <c r="E1011" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1011" s="9">
         <v>0</v>
@@ -30688,23 +30695,21 @@
       <c r="G1011" s="8">
         <v>0</v>
       </c>
-      <c r="H1011" s="6" t="s">
-        <v>1846</v>
-      </c>
+      <c r="H1011" s="6"/>
     </row>
     <row r="1012" spans="1:8">
       <c r="A1012" s="5" t="s">
+        <v>1846</v>
+      </c>
+      <c r="B1012" s="6" t="s">
         <v>1847</v>
       </c>
-      <c r="B1012" s="6" t="s">
-        <v>1848</v>
-      </c>
       <c r="C1012" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1012" s="6"/>
       <c r="E1012" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1012" s="9">
         <v>0</v>
@@ -30712,7 +30717,9 @@
       <c r="G1012" s="8">
         <v>0</v>
       </c>
-      <c r="H1012" s="6"/>
+      <c r="H1012" s="6" t="s">
+        <v>1848</v>
+      </c>
     </row>
     <row r="1013" spans="1:8">
       <c r="A1013" s="5" t="s">
@@ -30722,15 +30729,13 @@
         <v>1850</v>
       </c>
       <c r="C1013" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1013" s="5" t="s">
-        <v>1851</v>
-      </c>
+        <v>1828</v>
+      </c>
+      <c r="D1013" s="6"/>
       <c r="E1013" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1013" s="8">
+        <v>1828</v>
+      </c>
+      <c r="F1013" s="9">
         <v>0</v>
       </c>
       <c r="G1013" s="8">
@@ -30740,19 +30745,21 @@
     </row>
     <row r="1014" spans="1:8">
       <c r="A1014" s="5" t="s">
+        <v>1851</v>
+      </c>
+      <c r="B1014" s="6" t="s">
         <v>1852</v>
       </c>
-      <c r="B1014" s="6" t="s">
+      <c r="C1014" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1014" s="5" t="s">
         <v>1853</v>
       </c>
-      <c r="C1014" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1014" s="6"/>
       <c r="E1014" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1014" s="9">
+        <v>1828</v>
+      </c>
+      <c r="F1014" s="8">
         <v>0</v>
       </c>
       <c r="G1014" s="8">
@@ -30768,13 +30775,13 @@
         <v>1855</v>
       </c>
       <c r="C1015" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1015" s="6"/>
       <c r="E1015" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1015" s="8">
+        <v>1828</v>
+      </c>
+      <c r="F1015" s="9">
         <v>0</v>
       </c>
       <c r="G1015" s="8">
@@ -30786,41 +30793,41 @@
       <c r="A1016" s="5" t="s">
         <v>1856</v>
       </c>
-      <c r="B1016" s="5" t="s">
+      <c r="B1016" s="6" t="s">
         <v>1857</v>
       </c>
       <c r="C1016" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1016" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1016" s="6"/>
+      <c r="E1016" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F1016" s="8">
+        <v>0</v>
+      </c>
+      <c r="G1016" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1016" s="6"/>
+    </row>
+    <row r="1017" spans="1:8">
+      <c r="A1017" s="5" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B1017" s="5" t="s">
+        <v>1859</v>
+      </c>
+      <c r="C1017" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1017" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1016" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1016" s="9">
-        <v>0</v>
-      </c>
-      <c r="G1016" s="8">
-        <v>0</v>
-      </c>
-      <c r="H1016" s="6"/>
-    </row>
-    <row r="1017" spans="1:8">
-      <c r="A1017" s="6" t="s">
-        <v>1858</v>
-      </c>
-      <c r="B1017" s="6" t="s">
-        <v>1859</v>
-      </c>
-      <c r="C1017" s="6" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1017" s="6"/>
-      <c r="E1017" s="6" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1017" s="8">
+      <c r="E1017" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F1017" s="9">
         <v>0</v>
       </c>
       <c r="G1017" s="8">
@@ -30829,20 +30836,20 @@
       <c r="H1017" s="6"/>
     </row>
     <row r="1018" spans="1:8">
-      <c r="A1018" s="5" t="s">
+      <c r="A1018" s="6" t="s">
         <v>1860</v>
       </c>
       <c r="B1018" s="6" t="s">
         <v>1861</v>
       </c>
-      <c r="C1018" s="5" t="s">
-        <v>1826</v>
+      <c r="C1018" s="6" t="s">
+        <v>1828</v>
       </c>
       <c r="D1018" s="6"/>
-      <c r="E1018" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1018" s="9">
+      <c r="E1018" s="6" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F1018" s="8">
         <v>0</v>
       </c>
       <c r="G1018" s="8">
@@ -30858,13 +30865,11 @@
         <v>1863</v>
       </c>
       <c r="C1019" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1019" s="6" t="s">
-        <v>1864</v>
-      </c>
+        <v>1828</v>
+      </c>
+      <c r="D1019" s="6"/>
       <c r="E1019" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1019" s="9">
         <v>0</v>
@@ -30876,17 +30881,19 @@
     </row>
     <row r="1020" spans="1:8">
       <c r="A1020" s="5" t="s">
+        <v>1864</v>
+      </c>
+      <c r="B1020" s="6" t="s">
         <v>1865</v>
       </c>
-      <c r="B1020" s="5" t="s">
+      <c r="C1020" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1020" s="6" t="s">
         <v>1866</v>
       </c>
-      <c r="C1020" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1020" s="6"/>
       <c r="E1020" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1020" s="9">
         <v>0</v>
@@ -30904,11 +30911,11 @@
         <v>1868</v>
       </c>
       <c r="C1021" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1021" s="6"/>
       <c r="E1021" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1021" s="9">
         <v>0</v>
@@ -30923,16 +30930,16 @@
         <v>1869</v>
       </c>
       <c r="B1022" s="5" t="s">
-        <v>1868</v>
+        <v>1870</v>
       </c>
       <c r="C1022" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1022" s="6"/>
       <c r="E1022" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1022" s="8">
+        <v>1828</v>
+      </c>
+      <c r="F1022" s="9">
         <v>0</v>
       </c>
       <c r="G1022" s="8">
@@ -30942,19 +30949,17 @@
     </row>
     <row r="1023" spans="1:8">
       <c r="A1023" s="5" t="s">
+        <v>1871</v>
+      </c>
+      <c r="B1023" s="5" t="s">
         <v>1870</v>
       </c>
-      <c r="B1023" s="6" t="s">
-        <v>1871</v>
-      </c>
       <c r="C1023" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1023" s="5" t="s">
-        <v>1872</v>
-      </c>
+        <v>1828</v>
+      </c>
+      <c r="D1023" s="6"/>
       <c r="E1023" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1023" s="8">
         <v>0</v>
@@ -30966,19 +30971,21 @@
     </row>
     <row r="1024" spans="1:8">
       <c r="A1024" s="5" t="s">
+        <v>1872</v>
+      </c>
+      <c r="B1024" s="6" t="s">
         <v>1873</v>
       </c>
-      <c r="B1024" s="6" t="s">
+      <c r="C1024" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1024" s="5" t="s">
         <v>1874</v>
       </c>
-      <c r="C1024" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1024" s="6"/>
       <c r="E1024" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1024" s="9">
+        <v>1828</v>
+      </c>
+      <c r="F1024" s="8">
         <v>0</v>
       </c>
       <c r="G1024" s="8">
@@ -30994,13 +31001,13 @@
         <v>1876</v>
       </c>
       <c r="C1025" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1025" s="6"/>
       <c r="E1025" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1025" s="8">
+        <v>1828</v>
+      </c>
+      <c r="F1025" s="9">
         <v>0</v>
       </c>
       <c r="G1025" s="8">
@@ -31016,13 +31023,13 @@
         <v>1878</v>
       </c>
       <c r="C1026" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1026" s="6"/>
       <c r="E1026" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1026" s="9">
+        <v>1828</v>
+      </c>
+      <c r="F1026" s="8">
         <v>0</v>
       </c>
       <c r="G1026" s="8">
@@ -31038,13 +31045,11 @@
         <v>1880</v>
       </c>
       <c r="C1027" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1027" s="5" t="s">
-        <v>1881</v>
-      </c>
+        <v>1828</v>
+      </c>
+      <c r="D1027" s="6"/>
       <c r="E1027" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1027" s="9">
         <v>0</v>
@@ -31056,17 +31061,19 @@
     </row>
     <row r="1028" spans="1:8">
       <c r="A1028" s="5" t="s">
+        <v>1881</v>
+      </c>
+      <c r="B1028" s="6" t="s">
         <v>1882</v>
       </c>
-      <c r="B1028" s="6" t="s">
+      <c r="C1028" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1028" s="5" t="s">
         <v>1883</v>
       </c>
-      <c r="C1028" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1028" s="6"/>
       <c r="E1028" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1028" s="9">
         <v>0</v>
@@ -31074,47 +31081,47 @@
       <c r="G1028" s="8">
         <v>0</v>
       </c>
-      <c r="H1028" s="6" t="s">
-        <v>1884</v>
-      </c>
+      <c r="H1028" s="6"/>
     </row>
     <row r="1029" spans="1:8">
       <c r="A1029" s="5" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B1029" s="6" t="s">
         <v>1885</v>
       </c>
-      <c r="B1029" s="6" t="s">
+      <c r="C1029" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1029" s="6"/>
+      <c r="E1029" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F1029" s="9">
+        <v>0</v>
+      </c>
+      <c r="G1029" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1029" s="6" t="s">
         <v>1886</v>
       </c>
-      <c r="C1029" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1029" s="6" t="s">
-        <v>1887</v>
-      </c>
-      <c r="E1029" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1029" s="8">
-        <v>0</v>
-      </c>
-      <c r="G1029" s="8">
-        <v>0</v>
-      </c>
-      <c r="H1029" s="6"/>
     </row>
     <row r="1030" spans="1:8">
       <c r="A1030" s="5" t="s">
+        <v>1887</v>
+      </c>
+      <c r="B1030" s="6" t="s">
         <v>1888</v>
       </c>
-      <c r="B1030" s="6" t="s">
+      <c r="C1030" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1030" s="6" t="s">
         <v>1889</v>
       </c>
-      <c r="C1030" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1030" s="6"/>
       <c r="E1030" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1030" s="8">
         <v>0</v>
@@ -31132,13 +31139,13 @@
         <v>1891</v>
       </c>
       <c r="C1031" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1031" s="6"/>
       <c r="E1031" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1031" s="9">
+        <v>1828</v>
+      </c>
+      <c r="F1031" s="8">
         <v>0</v>
       </c>
       <c r="G1031" s="8">
@@ -31154,13 +31161,13 @@
         <v>1893</v>
       </c>
       <c r="C1032" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1032" s="6"/>
       <c r="E1032" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1032" s="8">
+        <v>1828</v>
+      </c>
+      <c r="F1032" s="9">
         <v>0</v>
       </c>
       <c r="G1032" s="8">
@@ -31172,15 +31179,15 @@
       <c r="A1033" s="5" t="s">
         <v>1894</v>
       </c>
-      <c r="B1033" s="5" t="s">
+      <c r="B1033" s="6" t="s">
         <v>1895</v>
       </c>
       <c r="C1033" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1033" s="6"/>
       <c r="E1033" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1033" s="8">
         <v>0</v>
@@ -31194,63 +31201,63 @@
       <c r="A1034" s="5" t="s">
         <v>1896</v>
       </c>
-      <c r="B1034" s="6" t="s">
+      <c r="B1034" s="5" t="s">
         <v>1897</v>
       </c>
       <c r="C1034" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1034" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1034" s="6"/>
+      <c r="E1034" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F1034" s="8">
+        <v>0</v>
+      </c>
+      <c r="G1034" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1034" s="6"/>
+    </row>
+    <row r="1035" spans="1:8">
+      <c r="A1035" s="5" t="s">
         <v>1898</v>
       </c>
-      <c r="E1034" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1034" s="9">
-        <v>0</v>
-      </c>
-      <c r="G1034" s="8">
-        <v>0</v>
-      </c>
-      <c r="H1034" s="6" t="s">
+      <c r="B1035" s="6" t="s">
         <v>1899</v>
       </c>
-    </row>
-    <row r="1035" spans="1:8">
-      <c r="A1035" s="6" t="s">
+      <c r="C1035" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1035" s="5" t="s">
         <v>1900</v>
       </c>
-      <c r="B1035" s="5" t="s">
+      <c r="E1035" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F1035" s="9">
+        <v>0</v>
+      </c>
+      <c r="G1035" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1035" s="6" t="s">
         <v>1901</v>
       </c>
-      <c r="C1035" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1035" s="6"/>
-      <c r="E1035" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1035" s="8">
-        <v>0</v>
-      </c>
-      <c r="G1035" s="8">
-        <v>0</v>
-      </c>
-      <c r="H1035" s="6"/>
     </row>
     <row r="1036" spans="1:8">
-      <c r="A1036" s="5" t="s">
+      <c r="A1036" s="6" t="s">
         <v>1902</v>
       </c>
       <c r="B1036" s="5" t="s">
         <v>1903</v>
       </c>
       <c r="C1036" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1036" s="6"/>
       <c r="E1036" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1036" s="8">
         <v>0</v>
@@ -31264,15 +31271,15 @@
       <c r="A1037" s="5" t="s">
         <v>1904</v>
       </c>
-      <c r="B1037" s="6" t="s">
+      <c r="B1037" s="5" t="s">
         <v>1905</v>
       </c>
       <c r="C1037" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1037" s="6"/>
       <c r="E1037" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1037" s="8">
         <v>0</v>
@@ -31290,13 +31297,13 @@
         <v>1907</v>
       </c>
       <c r="C1038" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1038" s="6"/>
       <c r="E1038" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1038" s="9">
+        <v>1828</v>
+      </c>
+      <c r="F1038" s="8">
         <v>0</v>
       </c>
       <c r="G1038" s="8">
@@ -31308,39 +31315,37 @@
       <c r="A1039" s="5" t="s">
         <v>1908</v>
       </c>
-      <c r="B1039" s="5" t="s">
+      <c r="B1039" s="6" t="s">
         <v>1909</v>
       </c>
       <c r="C1039" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1039" s="6"/>
       <c r="E1039" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1039" s="8">
+        <v>1828</v>
+      </c>
+      <c r="F1039" s="9">
         <v>0</v>
       </c>
       <c r="G1039" s="8">
         <v>0</v>
       </c>
-      <c r="H1039" s="6" t="s">
-        <v>1910</v>
-      </c>
+      <c r="H1039" s="6"/>
     </row>
     <row r="1040" spans="1:8">
       <c r="A1040" s="5" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B1040" s="5" t="s">
         <v>1911</v>
       </c>
-      <c r="B1040" s="6" t="s">
-        <v>1912</v>
-      </c>
       <c r="C1040" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1040" s="6"/>
       <c r="E1040" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1040" s="8">
         <v>0</v>
@@ -31348,7 +31353,9 @@
       <c r="G1040" s="8">
         <v>0</v>
       </c>
-      <c r="H1040" s="6"/>
+      <c r="H1040" s="6" t="s">
+        <v>1912</v>
+      </c>
     </row>
     <row r="1041" spans="1:8">
       <c r="A1041" s="5" t="s">
@@ -31358,43 +31365,43 @@
         <v>1914</v>
       </c>
       <c r="C1041" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1041" s="6"/>
       <c r="E1041" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1041" s="9">
+        <v>1828</v>
+      </c>
+      <c r="F1041" s="8">
         <v>0</v>
       </c>
       <c r="G1041" s="8">
         <v>0</v>
       </c>
-      <c r="H1041" s="6" t="s">
-        <v>1915</v>
-      </c>
+      <c r="H1041" s="6"/>
     </row>
     <row r="1042" spans="1:8">
       <c r="A1042" s="5" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B1042" s="6" t="s">
         <v>1916</v>
       </c>
-      <c r="B1042" s="5" t="s">
+      <c r="C1042" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1042" s="6"/>
+      <c r="E1042" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F1042" s="9">
+        <v>0</v>
+      </c>
+      <c r="G1042" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1042" s="6" t="s">
         <v>1917</v>
       </c>
-      <c r="C1042" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1042" s="5"/>
-      <c r="E1042" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1042" s="9">
-        <v>0</v>
-      </c>
-      <c r="G1042" s="8">
-        <v>0</v>
-      </c>
-      <c r="H1042" s="6"/>
     </row>
     <row r="1043" spans="1:8">
       <c r="A1043" s="5" t="s">
@@ -31404,11 +31411,11 @@
         <v>1919</v>
       </c>
       <c r="C1043" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1043" s="6"/>
+        <v>1828</v>
+      </c>
+      <c r="D1043" s="5"/>
       <c r="E1043" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1043" s="9">
         <v>0</v>
@@ -31426,13 +31433,13 @@
         <v>1921</v>
       </c>
       <c r="C1044" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1044" s="6"/>
       <c r="E1044" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1044" s="8">
+        <v>1828</v>
+      </c>
+      <c r="F1044" s="9">
         <v>0</v>
       </c>
       <c r="G1044" s="8">
@@ -31444,15 +31451,15 @@
       <c r="A1045" s="5" t="s">
         <v>1922</v>
       </c>
-      <c r="B1045" s="6" t="s">
+      <c r="B1045" s="5" t="s">
         <v>1923</v>
       </c>
       <c r="C1045" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1045" s="6"/>
       <c r="E1045" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1045" s="8">
         <v>0</v>
@@ -31463,20 +31470,20 @@
       <c r="H1045" s="6"/>
     </row>
     <row r="1046" spans="1:8">
-      <c r="A1046" s="35" t="s">
+      <c r="A1046" s="5" t="s">
         <v>1924</v>
       </c>
-      <c r="B1046" s="36" t="s">
+      <c r="B1046" s="6" t="s">
         <v>1925</v>
       </c>
       <c r="C1046" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1046" s="6"/>
       <c r="E1046" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1046" s="9">
+        <v>1828</v>
+      </c>
+      <c r="F1046" s="8">
         <v>0</v>
       </c>
       <c r="G1046" s="8">
@@ -31485,44 +31492,44 @@
       <c r="H1046" s="6"/>
     </row>
     <row r="1047" spans="1:8">
-      <c r="A1047" s="37" t="s">
+      <c r="A1047" s="35" t="s">
         <v>1926</v>
       </c>
-      <c r="B1047" s="5" t="s">
+      <c r="B1047" s="36" t="s">
         <v>1927</v>
       </c>
       <c r="C1047" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1047" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1047" s="6"/>
+      <c r="E1047" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F1047" s="9">
+        <v>0</v>
+      </c>
+      <c r="G1047" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1047" s="6"/>
+    </row>
+    <row r="1048" spans="1:8">
+      <c r="A1048" s="37" t="s">
         <v>1928</v>
       </c>
-      <c r="E1047" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1047" s="9">
-        <v>0</v>
-      </c>
-      <c r="G1047" s="8">
-        <v>0</v>
-      </c>
-      <c r="H1047" s="6"/>
-    </row>
-    <row r="1048" spans="1:8">
-      <c r="A1048" s="5" t="s">
+      <c r="B1048" s="5" t="s">
         <v>1929</v>
       </c>
-      <c r="B1048" s="6" t="s">
+      <c r="C1048" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1048" s="5" t="s">
         <v>1930</v>
       </c>
-      <c r="C1048" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1048" s="6"/>
       <c r="E1048" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1048" s="8">
+        <v>1828</v>
+      </c>
+      <c r="F1048" s="9">
         <v>0</v>
       </c>
       <c r="G1048" s="8">
@@ -31538,13 +31545,13 @@
         <v>1932</v>
       </c>
       <c r="C1049" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1049" s="6"/>
       <c r="E1049" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1049" s="9">
+        <v>1828</v>
+      </c>
+      <c r="F1049" s="8">
         <v>0</v>
       </c>
       <c r="G1049" s="8">
@@ -31560,13 +31567,13 @@
         <v>1934</v>
       </c>
       <c r="C1050" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1050" s="6"/>
       <c r="E1050" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1050" s="8">
+        <v>1828</v>
+      </c>
+      <c r="F1050" s="9">
         <v>0</v>
       </c>
       <c r="G1050" s="8">
@@ -31578,17 +31585,17 @@
       <c r="A1051" s="5" t="s">
         <v>1935</v>
       </c>
-      <c r="B1051" s="5" t="s">
+      <c r="B1051" s="6" t="s">
         <v>1936</v>
       </c>
       <c r="C1051" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1051" s="6"/>
       <c r="E1051" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1051" s="9">
+        <v>1828</v>
+      </c>
+      <c r="F1051" s="8">
         <v>0</v>
       </c>
       <c r="G1051" s="8">
@@ -31600,15 +31607,15 @@
       <c r="A1052" s="5" t="s">
         <v>1937</v>
       </c>
-      <c r="B1052" s="6" t="s">
+      <c r="B1052" s="5" t="s">
         <v>1938</v>
       </c>
       <c r="C1052" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1052" s="6"/>
       <c r="E1052" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1052" s="9">
         <v>0</v>
@@ -31622,19 +31629,17 @@
       <c r="A1053" s="5" t="s">
         <v>1939</v>
       </c>
-      <c r="B1053" s="5" t="s">
-        <v>1938</v>
+      <c r="B1053" s="6" t="s">
+        <v>1940</v>
       </c>
       <c r="C1053" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1053" s="5" t="s">
-        <v>1940</v>
-      </c>
+        <v>1828</v>
+      </c>
+      <c r="D1053" s="6"/>
       <c r="E1053" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1053" s="8">
+        <v>1828</v>
+      </c>
+      <c r="F1053" s="9">
         <v>0</v>
       </c>
       <c r="G1053" s="8">
@@ -31646,15 +31651,17 @@
       <c r="A1054" s="5" t="s">
         <v>1941</v>
       </c>
-      <c r="B1054" s="6" t="s">
+      <c r="B1054" s="5" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C1054" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1054" s="5" t="s">
         <v>1942</v>
       </c>
-      <c r="C1054" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1054" s="6"/>
       <c r="E1054" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1054" s="8">
         <v>0</v>
@@ -31662,23 +31669,21 @@
       <c r="G1054" s="8">
         <v>0</v>
       </c>
-      <c r="H1054" s="6" t="s">
-        <v>1943</v>
-      </c>
+      <c r="H1054" s="6"/>
     </row>
     <row r="1055" spans="1:8">
       <c r="A1055" s="5" t="s">
+        <v>1943</v>
+      </c>
+      <c r="B1055" s="6" t="s">
         <v>1944</v>
       </c>
-      <c r="B1055" s="5" t="s">
-        <v>1945</v>
-      </c>
       <c r="C1055" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1055" s="6"/>
       <c r="E1055" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1055" s="8">
         <v>0</v>
@@ -31686,23 +31691,23 @@
       <c r="G1055" s="8">
         <v>0</v>
       </c>
-      <c r="H1055" s="6"/>
+      <c r="H1055" s="6" t="s">
+        <v>1945</v>
+      </c>
     </row>
     <row r="1056" spans="1:8">
       <c r="A1056" s="5" t="s">
         <v>1946</v>
       </c>
       <c r="B1056" s="5" t="s">
-        <v>1945</v>
+        <v>1947</v>
       </c>
       <c r="C1056" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1056" s="5" t="s">
-        <v>1947</v>
-      </c>
+        <v>1828</v>
+      </c>
+      <c r="D1056" s="6"/>
       <c r="E1056" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1056" s="8">
         <v>0</v>
@@ -31710,49 +31715,49 @@
       <c r="G1056" s="8">
         <v>0</v>
       </c>
-      <c r="H1056" s="6" t="s">
-        <v>1948</v>
-      </c>
+      <c r="H1056" s="6"/>
     </row>
     <row r="1057" spans="1:8">
       <c r="A1057" s="5" t="s">
+        <v>1948</v>
+      </c>
+      <c r="B1057" s="5" t="s">
+        <v>1947</v>
+      </c>
+      <c r="C1057" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1057" s="5" t="s">
         <v>1949</v>
       </c>
-      <c r="B1057" s="5" t="s">
-        <v>1945</v>
-      </c>
-      <c r="C1057" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1057" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="E1057" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1057" s="9">
+        <v>1828</v>
+      </c>
+      <c r="F1057" s="8">
         <v>0</v>
       </c>
       <c r="G1057" s="8">
         <v>0</v>
       </c>
-      <c r="H1057" s="6"/>
+      <c r="H1057" s="6" t="s">
+        <v>1950</v>
+      </c>
     </row>
     <row r="1058" spans="1:8">
       <c r="A1058" s="5" t="s">
-        <v>1950</v>
+        <v>1951</v>
       </c>
       <c r="B1058" s="5" t="s">
-        <v>1945</v>
+        <v>1947</v>
       </c>
       <c r="C1058" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1058" s="5" t="s">
-        <v>1951</v>
+        <v>11</v>
       </c>
       <c r="E1058" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="F1058" s="9">
         <v>0</v>
@@ -31767,110 +31772,112 @@
         <v>1952</v>
       </c>
       <c r="B1059" s="5" t="s">
-        <v>1945</v>
+        <v>1947</v>
       </c>
       <c r="C1059" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1059" s="5" t="s">
+        <v>1953</v>
+      </c>
+      <c r="E1059" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F1059" s="9">
+        <v>0</v>
+      </c>
+      <c r="G1059" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1059" s="6"/>
+    </row>
+    <row r="1060" spans="1:8">
+      <c r="A1060" s="5" t="s">
+        <v>1954</v>
+      </c>
+      <c r="B1060" s="5" t="s">
+        <v>1947</v>
+      </c>
+      <c r="C1060" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D1060" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1059" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1059" s="8">
-        <v>0</v>
-      </c>
-      <c r="G1059" s="8">
-        <v>0</v>
-      </c>
-      <c r="H1059" s="6" t="s">
-        <v>1953</v>
-      </c>
-    </row>
-    <row r="1060" spans="1:8">
-      <c r="A1060" s="6" t="s">
-        <v>1954</v>
-      </c>
-      <c r="B1060" s="5" t="s">
+      <c r="E1060" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F1060" s="8">
+        <v>0</v>
+      </c>
+      <c r="G1060" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1060" s="6" t="s">
         <v>1955</v>
       </c>
-      <c r="C1060" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="D1060" s="6"/>
-      <c r="E1060" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1060" s="9">
-        <v>0</v>
-      </c>
-      <c r="G1060" s="8">
-        <v>0</v>
-      </c>
-      <c r="H1060" s="6"/>
     </row>
     <row r="1061" spans="1:8">
-      <c r="A1061" s="5" t="s">
+      <c r="A1061" s="6" t="s">
         <v>1956</v>
       </c>
       <c r="B1061" s="5" t="s">
-        <v>328</v>
+        <v>1957</v>
       </c>
       <c r="C1061" s="5" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="D1061" s="6"/>
       <c r="E1061" s="5" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F1061" s="8">
+        <v>1828</v>
+      </c>
+      <c r="F1061" s="9">
         <v>0</v>
       </c>
       <c r="G1061" s="8">
         <v>0</v>
       </c>
-      <c r="H1061" s="6" t="s">
-        <v>1957</v>
-      </c>
+      <c r="H1061" s="6"/>
     </row>
     <row r="1062" spans="1:8">
       <c r="A1062" s="5" t="s">
-        <v>449</v>
+        <v>1958</v>
       </c>
       <c r="B1062" s="5" t="s">
-        <v>450</v>
+        <v>328</v>
       </c>
       <c r="C1062" s="5" t="s">
-        <v>1958</v>
+        <v>1828</v>
       </c>
       <c r="D1062" s="6"/>
       <c r="E1062" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="F1062" s="9">
+        <v>1828</v>
+      </c>
+      <c r="F1062" s="8">
         <v>0</v>
       </c>
       <c r="G1062" s="8">
         <v>0</v>
       </c>
-      <c r="H1062" s="6"/>
+      <c r="H1062" s="6" t="s">
+        <v>1959</v>
+      </c>
     </row>
     <row r="1063" spans="1:8">
       <c r="A1063" s="5" t="s">
-        <v>1959</v>
+        <v>449</v>
       </c>
       <c r="B1063" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="C1063" s="5" t="s">
         <v>1960</v>
-      </c>
-      <c r="C1063" s="5" t="s">
-        <v>1958</v>
       </c>
       <c r="D1063" s="6"/>
       <c r="E1063" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="F1063" s="8">
+        <v>1960</v>
+      </c>
+      <c r="F1063" s="9">
         <v>0</v>
       </c>
       <c r="G1063" s="8">
@@ -31886,11 +31893,11 @@
         <v>1962</v>
       </c>
       <c r="C1064" s="5" t="s">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="D1064" s="6"/>
       <c r="E1064" s="5" t="s">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="F1064" s="8">
         <v>0</v>
@@ -31908,11 +31915,11 @@
         <v>1964</v>
       </c>
       <c r="C1065" s="5" t="s">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="D1065" s="6"/>
       <c r="E1065" s="5" t="s">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="F1065" s="8">
         <v>0</v>
@@ -31930,15 +31937,13 @@
         <v>1966</v>
       </c>
       <c r="C1066" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="D1066" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>1960</v>
+      </c>
+      <c r="D1066" s="6"/>
       <c r="E1066" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="F1066" s="9">
+        <v>1960</v>
+      </c>
+      <c r="F1066" s="8">
         <v>0</v>
       </c>
       <c r="G1066" s="8">
@@ -31951,16 +31956,16 @@
         <v>1967</v>
       </c>
       <c r="B1067" s="5" t="s">
-        <v>402</v>
+        <v>1968</v>
       </c>
       <c r="C1067" s="5" t="s">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="D1067" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E1067" s="5" t="s">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="F1067" s="9">
         <v>0</v>
@@ -31972,43 +31977,41 @@
     </row>
     <row r="1068" spans="1:8">
       <c r="A1068" s="5" t="s">
-        <v>1968</v>
+        <v>1969</v>
       </c>
       <c r="B1068" s="5" t="s">
         <v>402</v>
       </c>
       <c r="C1068" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="D1068" s="6"/>
+        <v>1960</v>
+      </c>
+      <c r="D1068" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E1068" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="F1068" s="8">
+        <v>1960</v>
+      </c>
+      <c r="F1068" s="9">
         <v>0</v>
       </c>
       <c r="G1068" s="8">
         <v>0</v>
       </c>
-      <c r="H1068" s="6" t="s">
-        <v>1969</v>
-      </c>
+      <c r="H1068" s="6"/>
     </row>
     <row r="1069" spans="1:8">
       <c r="A1069" s="5" t="s">
         <v>1970</v>
       </c>
       <c r="B1069" s="5" t="s">
-        <v>21</v>
+        <v>402</v>
       </c>
       <c r="C1069" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="D1069" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>1960</v>
+      </c>
+      <c r="D1069" s="6"/>
       <c r="E1069" s="5" t="s">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="F1069" s="8">
         <v>0</v>
@@ -32016,25 +32019,27 @@
       <c r="G1069" s="8">
         <v>0</v>
       </c>
-      <c r="H1069" s="6"/>
+      <c r="H1069" s="6" t="s">
+        <v>1971</v>
+      </c>
     </row>
     <row r="1070" spans="1:8">
       <c r="A1070" s="5" t="s">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="B1070" s="5" t="s">
-        <v>1972</v>
+        <v>21</v>
       </c>
       <c r="C1070" s="5" t="s">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="D1070" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E1070" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="F1070" s="9">
+        <v>1960</v>
+      </c>
+      <c r="F1070" s="8">
         <v>0</v>
       </c>
       <c r="G1070" s="8">
@@ -32050,13 +32055,13 @@
         <v>1974</v>
       </c>
       <c r="C1071" s="5" t="s">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="D1071" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E1071" s="5" t="s">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="F1071" s="9">
         <v>0</v>
@@ -32074,13 +32079,15 @@
         <v>1976</v>
       </c>
       <c r="C1072" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="D1072" s="6"/>
+        <v>1960</v>
+      </c>
+      <c r="D1072" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E1072" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="F1072" s="8">
+        <v>1960</v>
+      </c>
+      <c r="F1072" s="9">
         <v>0</v>
       </c>
       <c r="G1072" s="8">
@@ -32092,17 +32099,17 @@
       <c r="A1073" s="5" t="s">
         <v>1977</v>
       </c>
-      <c r="B1073" s="6" t="s">
+      <c r="B1073" s="5" t="s">
         <v>1978</v>
       </c>
       <c r="C1073" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="D1073" s="5"/>
+        <v>1960</v>
+      </c>
+      <c r="D1073" s="6"/>
       <c r="E1073" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="F1073" s="9">
+        <v>1960</v>
+      </c>
+      <c r="F1073" s="8">
         <v>0</v>
       </c>
       <c r="G1073" s="8">
@@ -32114,17 +32121,17 @@
       <c r="A1074" s="5" t="s">
         <v>1979</v>
       </c>
-      <c r="B1074" s="5" t="s">
+      <c r="B1074" s="6" t="s">
         <v>1980</v>
       </c>
       <c r="C1074" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="D1074" s="6"/>
+        <v>1960</v>
+      </c>
+      <c r="D1074" s="5"/>
       <c r="E1074" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="F1074" s="8">
+        <v>1960</v>
+      </c>
+      <c r="F1074" s="9">
         <v>0</v>
       </c>
       <c r="G1074" s="8">
@@ -32133,18 +32140,18 @@
       <c r="H1074" s="6"/>
     </row>
     <row r="1075" spans="1:8">
-      <c r="A1075" s="6" t="s">
+      <c r="A1075" s="5" t="s">
         <v>1981</v>
       </c>
-      <c r="B1075" s="6" t="s">
-        <v>1980</v>
-      </c>
-      <c r="C1075" s="6" t="s">
-        <v>1958</v>
+      <c r="B1075" s="5" t="s">
+        <v>1982</v>
+      </c>
+      <c r="C1075" s="5" t="s">
+        <v>1960</v>
       </c>
       <c r="D1075" s="6"/>
-      <c r="E1075" s="6" t="s">
-        <v>1958</v>
+      <c r="E1075" s="5" t="s">
+        <v>1960</v>
       </c>
       <c r="F1075" s="8">
         <v>0</v>
@@ -32155,18 +32162,18 @@
       <c r="H1075" s="6"/>
     </row>
     <row r="1076" spans="1:8">
-      <c r="A1076" s="5" t="s">
+      <c r="A1076" s="6" t="s">
+        <v>1983</v>
+      </c>
+      <c r="B1076" s="6" t="s">
         <v>1982</v>
       </c>
-      <c r="B1076" s="5" t="s">
-        <v>1983</v>
-      </c>
-      <c r="C1076" s="5" t="s">
-        <v>1958</v>
+      <c r="C1076" s="6" t="s">
+        <v>1960</v>
       </c>
       <c r="D1076" s="6"/>
-      <c r="E1076" s="5" t="s">
-        <v>1958</v>
+      <c r="E1076" s="6" t="s">
+        <v>1960</v>
       </c>
       <c r="F1076" s="8">
         <v>0</v>
@@ -32184,13 +32191,13 @@
         <v>1985</v>
       </c>
       <c r="C1077" s="5" t="s">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="D1077" s="6"/>
       <c r="E1077" s="5" t="s">
-        <v>1958</v>
-      </c>
-      <c r="F1077" s="9">
+        <v>1960</v>
+      </c>
+      <c r="F1077" s="8">
         <v>0</v>
       </c>
       <c r="G1077" s="8">
@@ -32199,18 +32206,18 @@
       <c r="H1077" s="6"/>
     </row>
     <row r="1078" spans="1:8">
-      <c r="A1078" t="s">
+      <c r="A1078" s="5" t="s">
         <v>1986</v>
       </c>
       <c r="B1078" s="5" t="s">
-        <v>1985</v>
+        <v>1987</v>
       </c>
       <c r="C1078" s="5" t="s">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="D1078" s="6"/>
       <c r="E1078" s="5" t="s">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="F1078" s="9">
         <v>0</v>
@@ -32220,18 +32227,37 @@
       </c>
       <c r="H1078" s="6"/>
     </row>
-    <row r="1079" spans="1:1">
-      <c r="A1079" s="11"/>
+    <row r="1079" spans="1:8">
+      <c r="A1079" t="s">
+        <v>1988</v>
+      </c>
+      <c r="B1079" s="5" t="s">
+        <v>1987</v>
+      </c>
+      <c r="C1079" s="5" t="s">
+        <v>1960</v>
+      </c>
+      <c r="D1079" s="6"/>
+      <c r="E1079" s="5" t="s">
+        <v>1960</v>
+      </c>
+      <c r="F1079" s="9">
+        <v>0</v>
+      </c>
+      <c r="G1079" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1079" s="6"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" insertHyperlinks="0" autoFilter="0"/>
   <autoFilter ref="A1:H1078">
-    <sortState ref="A2:H1078">
+    <sortState ref="A1:H1078">
       <sortCondition ref="E1"/>
     </sortState>
     <extLst/>
   </autoFilter>
-  <sortState ref="A2:H1063">
+  <sortState ref="A2:H1079">
     <sortCondition ref="E1"/>
   </sortState>
   <dataValidations count="1">
@@ -32243,7 +32269,7 @@
     <hyperlink ref="D930" r:id="rId1" display="《国王排名》ED" tooltip="https://baike.baidu.com/item/%E5%9B%BD%E7%8E%8B%E6%8E%92%E5%90%8D/24190907"/>
     <hyperlink ref="D207" r:id="rId2" display="《英雄联盟：双城之战》的中文主题曲" tooltip="https://baike.baidu.com/item/%E8%8B%B1%E9%9B%84%E8%81%94%E7%9B%9F%EF%BC%9A%E5%8F%8C%E5%9F%8E%E4%B9%8B%E6%88%98/58613563"/>
     <hyperlink ref="D900" r:id="rId3" display="我的世界已坠入爱河《闪烁的青春》OP主题曲" tooltip="https://baike.baidu.com/item/%E9%97%AA%E7%83%81%E7%9A%84%E9%9D%92%E6%98%A5/13320086"/>
-    <hyperlink ref="D990" r:id="rId4" display="《明日方舟》EP" tooltip="https://baike.baidu.com/item/%E9%AC%BC%E7%81%AD%E4%B9%8B%E5%88%83%EF%BC%9A%E6%97%A0%E9%99%90%E5%88%97%E8%BD%A6%E7%AF%87/23783245"/>
+    <hyperlink ref="D991" r:id="rId4" display="《明日方舟》EP" tooltip="https://baike.baidu.com/item/%E9%AC%BC%E7%81%AD%E4%B9%8B%E5%88%83%EF%BC%9A%E6%97%A0%E9%99%90%E5%88%97%E8%BD%A6%E7%AF%87/23783245"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -32253,8 +32279,8 @@
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <autofilters xmlns="https://web.wps.cn/et/2018/main">
   <sheetItem sheetStid="1">
+    <filterData filterID="1331220589"/>
     <filterData filterID="1331040869"/>
-    <filterData filterID="1331220589"/>
     <autofilterInfo filterID="1331040869">
       <autoFilter xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1078"/>
     </autofilterInfo>

</xml_diff>

<commit_message>
updated song list 2022/3/7
</commit_message>
<xml_diff>
--- a/music_list_7.xlsx
+++ b/music_list_7.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$1079</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$1084</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4932" uniqueCount="1995">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4954" uniqueCount="2004">
   <si>
     <t>歌名</t>
   </si>
@@ -5461,7 +5461,7 @@
     <t>さよならのこと</t>
   </si>
   <si>
-    <t>《WHITE Album》</t>
+    <t>《白色相簿》《WHITE Album》</t>
   </si>
   <si>
     <t>扉を開けて/敞开心扉</t>
@@ -6059,6 +6059,33 @@
   </si>
   <si>
     <t>少女的祈祷</t>
+  </si>
+  <si>
+    <t>逆さまの蝶</t>
+  </si>
+  <si>
+    <t>SNoW</t>
+  </si>
+  <si>
+    <t>TV动画《地狱少女》op</t>
+  </si>
+  <si>
+    <t>Pierce</t>
+  </si>
+  <si>
+    <t>桜色舞うころ</t>
+  </si>
+  <si>
+    <t>樱花樱花想见你</t>
+  </si>
+  <si>
+    <t>RSP</t>
+  </si>
+  <si>
+    <t>深爱</t>
+  </si>
+  <si>
+    <t>水树奈奈</t>
   </si>
 </sst>
 </file>
@@ -6066,44 +6093,44 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="39">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
     <numFmt numFmtId="176" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="#\ ??/??"/>
+    <numFmt numFmtId="178" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="179" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="180" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
+    <numFmt numFmtId="182" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="183" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="184" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="185" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
+    <numFmt numFmtId="186" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="187" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="188" formatCode="m/d"/>
+    <numFmt numFmtId="189" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="190" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="191" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
+    <numFmt numFmtId="192" formatCode="mmmmm\-yy"/>
+    <numFmt numFmtId="193" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="194" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="195" formatCode="#\ ??"/>
+    <numFmt numFmtId="196" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
+    <numFmt numFmtId="197" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="198" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
     <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="178" formatCode="[$-804]aaa"/>
-    <numFmt numFmtId="179" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="181" formatCode="m/d"/>
-    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="182" formatCode="yy/m/d"/>
-    <numFmt numFmtId="183" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="184" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="185" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="186" formatCode="mmmmm"/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="187" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="188" formatCode="mmmm\-yy"/>
-    <numFmt numFmtId="189" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="190" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="191" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
-    <numFmt numFmtId="192" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="193" formatCode="#\ ?/?"/>
-    <numFmt numFmtId="194" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
-    <numFmt numFmtId="195" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="196" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="197" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="198" formatCode="#\ ??"/>
-    <numFmt numFmtId="199" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="199" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
     <numFmt numFmtId="200" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="201" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="202" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
-    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="201" formatCode="mmmmm"/>
+    <numFmt numFmtId="202" formatCode="yy/m/d"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="47">
@@ -6286,11 +6313,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6302,30 +6328,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -6339,9 +6343,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6357,29 +6391,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6394,16 +6406,15 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6417,19 +6428,35 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10.5"/>
       <color rgb="FF222222"/>
       <name val="initial"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="10.5"/>
       <color rgb="FF222222"/>
       <name val="initial"/>
@@ -6451,7 +6478,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6463,31 +6514,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6499,7 +6538,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6511,127 +6658,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6658,7 +6685,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6667,7 +6694,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6702,21 +6729,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -6742,150 +6754,165 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="192" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="197" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -6899,7 +6926,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -6917,10 +6944,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="194" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="191" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
@@ -7326,12 +7353,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1079"/>
+  <dimension ref="A1:H1084"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A900" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B1079" sqref="B1079"/>
+      <selection pane="bottomLeft" activeCell="A1082" sqref="A1082"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -9038,7 +9065,7 @@
         <v>85</v>
       </c>
       <c r="F72" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G72" s="2">
         <v>0</v>
@@ -13790,7 +13817,7 @@
         <v>447</v>
       </c>
       <c r="F276" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G276" s="2">
         <v>0</v>
@@ -14772,7 +14799,7 @@
         <v>541</v>
       </c>
       <c r="F319" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G319" s="2">
         <v>0</v>
@@ -26115,7 +26142,7 @@
         <v>1320</v>
       </c>
       <c r="F812" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G812" s="2">
         <v>0</v>
@@ -28036,7 +28063,7 @@
         <v>1545</v>
       </c>
       <c r="F896" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G896" s="2">
         <v>0</v>
@@ -28059,7 +28086,7 @@
         <v>1545</v>
       </c>
       <c r="F897" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G897" s="2">
         <v>0</v>
@@ -28551,7 +28578,7 @@
         <v>1545</v>
       </c>
       <c r="F918" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G918" s="2">
         <v>0</v>
@@ -29086,7 +29113,7 @@
         <v>1545</v>
       </c>
       <c r="F941" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G941" s="2">
         <v>0</v>
@@ -29341,7 +29368,7 @@
         <v>1545</v>
       </c>
       <c r="F952" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G952" s="2">
         <v>0</v>
@@ -30167,7 +30194,7 @@
         <v>1545</v>
       </c>
       <c r="F987" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G987" s="2">
         <v>0</v>
@@ -32282,10 +32309,116 @@
       </c>
       <c r="H1079" s="6"/>
     </row>
+    <row r="1080" spans="1:7">
+      <c r="A1080" s="11" t="s">
+        <v>1995</v>
+      </c>
+      <c r="B1080" s="11" t="s">
+        <v>1996</v>
+      </c>
+      <c r="C1080" s="11" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D1080" s="11" t="s">
+        <v>1997</v>
+      </c>
+      <c r="E1080" s="11" t="s">
+        <v>1545</v>
+      </c>
+      <c r="F1080" s="2">
+        <v>1</v>
+      </c>
+      <c r="G1080" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:7">
+      <c r="A1081" s="11" t="s">
+        <v>1998</v>
+      </c>
+      <c r="B1081" s="11" t="s">
+        <v>1626</v>
+      </c>
+      <c r="C1081" s="11" t="s">
+        <v>1545</v>
+      </c>
+      <c r="E1081" s="11" t="s">
+        <v>1545</v>
+      </c>
+      <c r="F1081" s="2">
+        <v>1</v>
+      </c>
+      <c r="G1081" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:7">
+      <c r="A1082" s="11" t="s">
+        <v>1999</v>
+      </c>
+      <c r="B1082" s="11" t="s">
+        <v>1828</v>
+      </c>
+      <c r="C1082" s="11" t="s">
+        <v>1545</v>
+      </c>
+      <c r="E1082" s="11" t="s">
+        <v>1545</v>
+      </c>
+      <c r="F1082" s="2">
+        <v>1</v>
+      </c>
+      <c r="G1082" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:7">
+      <c r="A1083" s="11" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B1083" s="11" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C1083" s="11" t="s">
+        <v>1545</v>
+      </c>
+      <c r="E1083" s="11" t="s">
+        <v>1545</v>
+      </c>
+      <c r="F1083" s="2">
+        <v>1</v>
+      </c>
+      <c r="G1083" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:7">
+      <c r="A1084" s="11" t="s">
+        <v>2002</v>
+      </c>
+      <c r="B1084" s="11" t="s">
+        <v>2003</v>
+      </c>
+      <c r="C1084" s="11" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D1084" s="11" t="s">
+        <v>1795</v>
+      </c>
+      <c r="E1084" s="11" t="s">
+        <v>1545</v>
+      </c>
+      <c r="F1084" s="2">
+        <v>1</v>
+      </c>
+      <c r="G1084" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" insertHyperlinks="0" autoFilter="0"/>
-  <autoFilter ref="A1:H1079">
-    <sortState ref="A1:H1079">
+  <autoFilter ref="A1:H1084">
+    <sortState ref="A1:H1084">
       <sortCondition ref="E1"/>
     </sortState>
     <extLst/>
@@ -32312,10 +32445,27 @@
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <autofilters xmlns="https://web.wps.cn/et/2018/main">
   <sheetItem sheetStid="1">
-    <filterData filterID="1331040869"/>
+    <filterData filterID="1331040869">
+      <hiddenRange rowFrom="1" rowTo="70"/>
+      <hiddenRange rowFrom="72" rowTo="274"/>
+      <hiddenRange rowFrom="276" rowTo="317"/>
+      <hiddenRange rowFrom="319" rowTo="810"/>
+      <hiddenRange rowFrom="812" rowTo="894"/>
+      <hiddenRange rowFrom="897" rowTo="916"/>
+      <hiddenRange rowFrom="918" rowTo="939"/>
+      <hiddenRange rowFrom="941" rowTo="950"/>
+      <hiddenRange rowFrom="952" rowTo="985"/>
+      <hiddenRange rowFrom="987" rowTo="1078"/>
+    </filterData>
     <filterData filterID="1331220589"/>
     <autofilterInfo filterID="1331040869">
-      <autoFilter xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1079"/>
+      <autoFilter xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1084">
+        <filterColumn colId="5">
+          <customFilters>
+            <customFilter operator="equal" val="☑"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
     </autofilterInfo>
   </sheetItem>
 </autofilters>

</xml_diff>

<commit_message>
v1.4.0 update along with previous commit, finalized song list
</commit_message>
<xml_diff>
--- a/music_list_7.xlsx
+++ b/music_list_7.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5200" uniqueCount="2102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5204" uniqueCount="2103">
   <si>
     <t>歌名</t>
   </si>
@@ -6295,6 +6295,9 @@
     <t>BV143411K7SJ</t>
   </si>
   <si>
+    <t>Wake</t>
+  </si>
+  <si>
     <t>粤语</t>
   </si>
   <si>
@@ -6387,45 +6390,45 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="39">
-    <numFmt numFmtId="176" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="177" formatCode="mmmm\-yy"/>
-    <numFmt numFmtId="178" formatCode="#\ ??/??"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
+    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
+    <numFmt numFmtId="177" formatCode="#\ ??/??"/>
+    <numFmt numFmtId="178" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="179" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="180" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="181" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="182" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="183" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="184" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
+    <numFmt numFmtId="185" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="186" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="187" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="188" formatCode="yy/m/d"/>
     <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="179" formatCode="#\ ?/?"/>
-    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
+    <numFmt numFmtId="189" formatCode="m/d"/>
+    <numFmt numFmtId="190" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="191" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="192" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="193" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="194" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="195" formatCode="mmmmm"/>
+    <numFmt numFmtId="196" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
     <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="180" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="181" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="182" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="183" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="184" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="185" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="186" formatCode="mmmmm"/>
-    <numFmt numFmtId="187" formatCode="yy/m/d"/>
-    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
-    <numFmt numFmtId="188" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="189" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="190" formatCode="m/d"/>
-    <numFmt numFmtId="191" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="192" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
-    <numFmt numFmtId="193" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="194" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="195" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="196" formatCode="#\ ??"/>
-    <numFmt numFmtId="197" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="197" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
+    <numFmt numFmtId="198" formatCode="#\ ??"/>
+    <numFmt numFmtId="199" formatCode="\¥#,##0;\¥\-#,##0"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="198" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="199" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="200" formatCode="[$-804]aaa"/>
-    <numFmt numFmtId="201" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="202" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="200" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="201" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="202" formatCode="mmmmm\-yy"/>
   </numFmts>
   <fonts count="47">
     <font>
@@ -6601,7 +6604,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6615,7 +6618,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -6630,11 +6633,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6645,25 +6647,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6672,22 +6660,6 @@
       <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6702,6 +6674,46 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6728,19 +6740,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6772,13 +6775,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6790,13 +6847,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6808,127 +6859,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6952,7 +6889,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6969,8 +6972,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6980,41 +6983,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7063,129 +7031,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="192" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -7194,22 +7197,22 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7220,7 +7223,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="197" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -7238,10 +7241,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="197" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="197" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
@@ -7650,7 +7653,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1133"/>
+  <dimension ref="A1:H1134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A780" activePane="bottomLeft" state="frozen"/>
@@ -33446,43 +33449,42 @@
         <v>2072</v>
       </c>
     </row>
-    <row r="1117" spans="1:8">
-      <c r="A1117" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="B1117" s="5" t="s">
-        <v>457</v>
-      </c>
-      <c r="C1117" s="5" t="s">
+    <row r="1117" spans="1:7">
+      <c r="A1117" s="11" t="s">
         <v>2073</v>
       </c>
-      <c r="D1117" s="6"/>
-      <c r="E1117" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="F1117" s="9">
-        <v>0</v>
-      </c>
-      <c r="G1117" s="8">
-        <v>0</v>
-      </c>
-      <c r="H1117" s="6"/>
+      <c r="B1117" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C1117" s="11" t="s">
+        <v>1941</v>
+      </c>
+      <c r="D1117" s="11"/>
+      <c r="E1117" s="11" t="s">
+        <v>1941</v>
+      </c>
+      <c r="F1117" s="2">
+        <v>1</v>
+      </c>
+      <c r="G1117" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="1118" spans="1:8">
       <c r="A1118" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="B1118" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="C1118" s="5" t="s">
         <v>2074</v>
-      </c>
-      <c r="B1118" s="5" t="s">
-        <v>2075</v>
-      </c>
-      <c r="C1118" s="5" t="s">
-        <v>2073</v>
       </c>
       <c r="D1118" s="6"/>
       <c r="E1118" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="F1118" s="8">
+        <v>2074</v>
+      </c>
+      <c r="F1118" s="9">
         <v>0</v>
       </c>
       <c r="G1118" s="8">
@@ -33492,17 +33494,17 @@
     </row>
     <row r="1119" spans="1:8">
       <c r="A1119" s="5" t="s">
+        <v>2075</v>
+      </c>
+      <c r="B1119" s="5" t="s">
         <v>2076</v>
       </c>
-      <c r="B1119" s="5" t="s">
-        <v>2077</v>
-      </c>
       <c r="C1119" s="5" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="D1119" s="6"/>
       <c r="E1119" s="5" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="F1119" s="8">
         <v>0</v>
@@ -33514,17 +33516,17 @@
     </row>
     <row r="1120" spans="1:8">
       <c r="A1120" s="5" t="s">
+        <v>2077</v>
+      </c>
+      <c r="B1120" s="5" t="s">
         <v>2078</v>
       </c>
-      <c r="B1120" s="5" t="s">
-        <v>2079</v>
-      </c>
       <c r="C1120" s="5" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="D1120" s="6"/>
       <c r="E1120" s="5" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="F1120" s="8">
         <v>0</v>
@@ -33536,21 +33538,19 @@
     </row>
     <row r="1121" spans="1:8">
       <c r="A1121" s="5" t="s">
+        <v>2079</v>
+      </c>
+      <c r="B1121" s="5" t="s">
         <v>2080</v>
       </c>
-      <c r="B1121" s="5" t="s">
-        <v>2081</v>
-      </c>
       <c r="C1121" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="D1121" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>2074</v>
+      </c>
+      <c r="D1121" s="6"/>
       <c r="E1121" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="F1121" s="9">
+        <v>2074</v>
+      </c>
+      <c r="F1121" s="8">
         <v>0</v>
       </c>
       <c r="G1121" s="8">
@@ -33560,19 +33560,19 @@
     </row>
     <row r="1122" spans="1:8">
       <c r="A1122" s="5" t="s">
+        <v>2081</v>
+      </c>
+      <c r="B1122" s="5" t="s">
         <v>2082</v>
       </c>
-      <c r="B1122" s="5" t="s">
-        <v>409</v>
-      </c>
       <c r="C1122" s="5" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="D1122" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E1122" s="5" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="F1122" s="9">
         <v>0</v>
@@ -33590,63 +33590,63 @@
         <v>409</v>
       </c>
       <c r="C1123" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="D1123" s="6"/>
+        <v>2074</v>
+      </c>
+      <c r="D1123" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E1123" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="F1123" s="8">
+        <v>2074</v>
+      </c>
+      <c r="F1123" s="9">
         <v>0</v>
       </c>
       <c r="G1123" s="8">
         <v>0</v>
       </c>
-      <c r="H1123" s="6" t="s">
-        <v>2084</v>
-      </c>
+      <c r="H1123" s="6"/>
     </row>
     <row r="1124" spans="1:8">
       <c r="A1124" s="5" t="s">
+        <v>2084</v>
+      </c>
+      <c r="B1124" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1124" s="5" t="s">
+        <v>2074</v>
+      </c>
+      <c r="D1124" s="6"/>
+      <c r="E1124" s="5" t="s">
+        <v>2074</v>
+      </c>
+      <c r="F1124" s="8">
+        <v>0</v>
+      </c>
+      <c r="G1124" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1124" s="6" t="s">
         <v>2085</v>
       </c>
-      <c r="B1124" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1124" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="D1124" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1124" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="F1124" s="8">
-        <v>0</v>
-      </c>
-      <c r="G1124" s="8">
-        <v>0</v>
-      </c>
-      <c r="H1124" s="6"/>
     </row>
     <row r="1125" spans="1:8">
       <c r="A1125" s="5" t="s">
         <v>2086</v>
       </c>
       <c r="B1125" s="5" t="s">
-        <v>2087</v>
+        <v>22</v>
       </c>
       <c r="C1125" s="5" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="D1125" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E1125" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="F1125" s="9">
+        <v>2074</v>
+      </c>
+      <c r="F1125" s="8">
         <v>0</v>
       </c>
       <c r="G1125" s="8">
@@ -33656,19 +33656,19 @@
     </row>
     <row r="1126" spans="1:8">
       <c r="A1126" s="5" t="s">
+        <v>2087</v>
+      </c>
+      <c r="B1126" s="5" t="s">
         <v>2088</v>
       </c>
-      <c r="B1126" s="5" t="s">
-        <v>2089</v>
-      </c>
       <c r="C1126" s="5" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="D1126" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E1126" s="5" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="F1126" s="9">
         <v>0</v>
@@ -33680,19 +33680,21 @@
     </row>
     <row r="1127" spans="1:8">
       <c r="A1127" s="5" t="s">
+        <v>2089</v>
+      </c>
+      <c r="B1127" s="5" t="s">
         <v>2090</v>
       </c>
-      <c r="B1127" s="5" t="s">
-        <v>2091</v>
-      </c>
       <c r="C1127" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="D1127" s="6"/>
+        <v>2074</v>
+      </c>
+      <c r="D1127" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E1127" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="F1127" s="8">
+        <v>2074</v>
+      </c>
+      <c r="F1127" s="9">
         <v>0</v>
       </c>
       <c r="G1127" s="8">
@@ -33702,19 +33704,19 @@
     </row>
     <row r="1128" spans="1:8">
       <c r="A1128" s="5" t="s">
+        <v>2091</v>
+      </c>
+      <c r="B1128" s="5" t="s">
         <v>2092</v>
       </c>
-      <c r="B1128" s="6" t="s">
-        <v>2093</v>
-      </c>
       <c r="C1128" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="D1128" s="5"/>
+        <v>2074</v>
+      </c>
+      <c r="D1128" s="6"/>
       <c r="E1128" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="F1128" s="9">
+        <v>2074</v>
+      </c>
+      <c r="F1128" s="8">
         <v>0</v>
       </c>
       <c r="G1128" s="8">
@@ -33724,39 +33726,39 @@
     </row>
     <row r="1129" spans="1:8">
       <c r="A1129" s="5" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B1129" s="6" t="s">
         <v>2094</v>
       </c>
-      <c r="B1129" s="5" t="s">
+      <c r="C1129" s="5" t="s">
+        <v>2074</v>
+      </c>
+      <c r="D1129" s="5"/>
+      <c r="E1129" s="5" t="s">
+        <v>2074</v>
+      </c>
+      <c r="F1129" s="9">
+        <v>0</v>
+      </c>
+      <c r="G1129" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1129" s="6"/>
+    </row>
+    <row r="1130" spans="1:8">
+      <c r="A1130" s="5" t="s">
         <v>2095</v>
       </c>
-      <c r="C1129" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="D1129" s="6"/>
-      <c r="E1129" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="F1129" s="8">
-        <v>0</v>
-      </c>
-      <c r="G1129" s="8">
-        <v>0</v>
-      </c>
-      <c r="H1129" s="6"/>
-    </row>
-    <row r="1130" spans="1:8">
-      <c r="A1130" s="6" t="s">
+      <c r="B1130" s="5" t="s">
         <v>2096</v>
       </c>
-      <c r="B1130" s="6" t="s">
-        <v>2095</v>
-      </c>
-      <c r="C1130" s="6" t="s">
-        <v>2073</v>
+      <c r="C1130" s="5" t="s">
+        <v>2074</v>
       </c>
       <c r="D1130" s="6"/>
-      <c r="E1130" s="6" t="s">
-        <v>2073</v>
+      <c r="E1130" s="5" t="s">
+        <v>2074</v>
       </c>
       <c r="F1130" s="8">
         <v>0</v>
@@ -33767,18 +33769,18 @@
       <c r="H1130" s="6"/>
     </row>
     <row r="1131" spans="1:8">
-      <c r="A1131" s="5" t="s">
+      <c r="A1131" s="6" t="s">
         <v>2097</v>
       </c>
-      <c r="B1131" s="5" t="s">
-        <v>2098</v>
-      </c>
-      <c r="C1131" s="5" t="s">
-        <v>2073</v>
+      <c r="B1131" s="6" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C1131" s="6" t="s">
+        <v>2074</v>
       </c>
       <c r="D1131" s="6"/>
-      <c r="E1131" s="5" t="s">
-        <v>2073</v>
+      <c r="E1131" s="6" t="s">
+        <v>2074</v>
       </c>
       <c r="F1131" s="8">
         <v>0</v>
@@ -33790,19 +33792,19 @@
     </row>
     <row r="1132" spans="1:8">
       <c r="A1132" s="5" t="s">
+        <v>2098</v>
+      </c>
+      <c r="B1132" s="5" t="s">
         <v>2099</v>
       </c>
-      <c r="B1132" s="5" t="s">
-        <v>2100</v>
-      </c>
       <c r="C1132" s="5" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="D1132" s="6"/>
       <c r="E1132" s="5" t="s">
-        <v>2073</v>
-      </c>
-      <c r="F1132" s="9">
+        <v>2074</v>
+      </c>
+      <c r="F1132" s="8">
         <v>0</v>
       </c>
       <c r="G1132" s="8">
@@ -33811,18 +33813,18 @@
       <c r="H1132" s="6"/>
     </row>
     <row r="1133" spans="1:8">
-      <c r="A1133" t="s">
+      <c r="A1133" s="5" t="s">
+        <v>2100</v>
+      </c>
+      <c r="B1133" s="5" t="s">
         <v>2101</v>
       </c>
-      <c r="B1133" s="5" t="s">
-        <v>2100</v>
-      </c>
       <c r="C1133" s="5" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="D1133" s="6"/>
       <c r="E1133" s="5" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="F1133" s="9">
         <v>0</v>
@@ -33831,6 +33833,28 @@
         <v>0</v>
       </c>
       <c r="H1133" s="6"/>
+    </row>
+    <row r="1134" spans="1:8">
+      <c r="A1134" t="s">
+        <v>2102</v>
+      </c>
+      <c r="B1134" s="5" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C1134" s="5" t="s">
+        <v>2074</v>
+      </c>
+      <c r="D1134" s="6"/>
+      <c r="E1134" s="5" t="s">
+        <v>2074</v>
+      </c>
+      <c r="F1134" s="9">
+        <v>0</v>
+      </c>
+      <c r="G1134" s="8">
+        <v>0</v>
+      </c>
+      <c r="H1134" s="6"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" insertHyperlinks="0" autoFilter="0"/>
@@ -33838,15 +33862,16 @@
     <protectedRange sqref="A$1:H$1048576" name="Range1"/>
   </protectedRanges>
   <autoFilter ref="A1:H1133">
-    <sortState ref="A2:H1133">
+    <sortState ref="A1:H1133">
       <sortCondition ref="E5"/>
     </sortState>
+    <extLst/>
   </autoFilter>
-  <sortState ref="A2:H1087">
+  <sortState ref="A2:H1134">
     <sortCondition ref="E1"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="输入内容有误" error="请选择勾选或取消勾选" sqref="F2:G1048576">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="输入内容有误" error="请选择勾选或取消勾选" sqref="F1134:G1134 F2:G1133 F1135:G1048576">
       <formula1>IF(TRUE,OR(F2=0,F2=1),"Checkbox")</formula1>
     </dataValidation>
   </dataValidations>
@@ -33877,8 +33902,8 @@
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <autofilters xmlns="https://web.wps.cn/et/2018/main">
   <sheetItem sheetStid="1">
+    <filterData filterID="1331220589"/>
     <filterData filterID="1331040869"/>
-    <filterData filterID="1331220589"/>
     <autofilterInfo filterID="1331040869">
       <autoFilter xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1133"/>
     </autofilterInfo>

</xml_diff>